<commit_message>
New data handling and updated technology list
</commit_message>
<xml_diff>
--- a/ConfigFiles/ConfigTest.xlsx
+++ b/ConfigFiles/ConfigTest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matij\Documents\Github\Heating\Heat-Markets\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00C04A7B-FC1A-451C-8472-9F59441CB397}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D62990BB-4C68-4AEF-BAC7-B358FC85249C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23055" yWindow="2340" windowWidth="16890" windowHeight="9915" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -527,10 +527,10 @@
     <t>Players - Supply Side</t>
   </si>
   <si>
-    <t>Database/Players/##/DemandSide.csv</t>
-  </si>
-  <si>
-    <t>Database/Players/##/SupplySide.csv</t>
+    <t>Database/Players/DemandSide/##/DemandSide.csv</t>
+  </si>
+  <si>
+    <t>Database/Players/SupplySide/##/SupplySide.csv</t>
   </si>
 </sst>
 </file>
@@ -1054,7 +1054,7 @@
   <dimension ref="A1:H165"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="C85" sqref="C85"/>
+      <selection activeCell="C71" sqref="C71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Model formulation now includes inter-zonal bids
</commit_message>
<xml_diff>
--- a/ConfigFiles/ConfigTest.xlsx
+++ b/ConfigFiles/ConfigTest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matij\Documents\Github\Heating\Heat-Markets\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D62990BB-4C68-4AEF-BAC7-B358FC85249C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB5EF2D9-D2B5-40B9-B4D1-44FE9BE70A3F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23055" yWindow="2340" windowWidth="16890" windowHeight="9915" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="159">
   <si>
     <t>Default value</t>
   </si>
@@ -209,9 +209,6 @@
     <t>it can be skipped.</t>
   </si>
   <si>
-    <t xml:space="preserve">For datasets which have one file per country, replace the country code (2 characters) in the path by ##. </t>
-  </si>
-  <si>
     <t>Date and time parameters of the simulation</t>
   </si>
   <si>
@@ -239,21 +236,6 @@
     <t>The specified factor scales up or down the capacity and the generation of the specified technology</t>
   </si>
   <si>
-    <t>Capacity Correction</t>
-  </si>
-  <si>
-    <t>Add plants</t>
-  </si>
-  <si>
-    <t>Scale-up capacities</t>
-  </si>
-  <si>
-    <t>Ignore</t>
-  </si>
-  <si>
-    <t>Display Warning</t>
-  </si>
-  <si>
     <t>GAMS path</t>
   </si>
   <si>
@@ -419,9 +401,6 @@
     <t>XK</t>
   </si>
   <si>
-    <t>AL</t>
-  </si>
-  <si>
     <t>IS</t>
   </si>
   <si>
@@ -458,9 +437,6 @@
     <t>This section defines the output of the pre-processing (which is the input of the DARKO solver)</t>
   </si>
   <si>
-    <t>Quantity - Block Order</t>
-  </si>
-  <si>
     <t>Price - Block Order</t>
   </si>
   <si>
@@ -476,12 +452,6 @@
     <t>!TODO</t>
   </si>
   <si>
-    <t xml:space="preserve">Quantity - Demand Order </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quantity - Simple Order </t>
-  </si>
-  <si>
     <t>Price - Demand Order</t>
   </si>
   <si>
@@ -491,36 +461,9 @@
     <t>Z1</t>
   </si>
   <si>
-    <t>Database/Quantity/##/Demand.csv</t>
-  </si>
-  <si>
-    <t>Database/Quantity/##/Supply.csv</t>
-  </si>
-  <si>
-    <t>Database/Quantity/##/BlockOrder.csv</t>
-  </si>
-  <si>
-    <t>Database/Price/##/Demand.csv</t>
-  </si>
-  <si>
-    <t>Database/Price/##/Supply.csv</t>
-  </si>
-  <si>
-    <t>Database/Price/##/BlockOrder.csv</t>
-  </si>
-  <si>
-    <t>Quantity - Flexible Order</t>
-  </si>
-  <si>
-    <t>Database/Quantity/##/FlexibleOrder.csv</t>
-  </si>
-  <si>
     <t>Price - Flexible Order</t>
   </si>
   <si>
-    <t>Database/Price/##/FlexibleOrder.csv</t>
-  </si>
-  <si>
     <t>Players - Demand Side</t>
   </si>
   <si>
@@ -531,6 +474,39 @@
   </si>
   <si>
     <t>Database/Players/SupplySide/##/SupplySide.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Availability - Demand Order </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Availability - Simple Order </t>
+  </si>
+  <si>
+    <t>Availability - Block Order</t>
+  </si>
+  <si>
+    <t>Availability - Flexible Order</t>
+  </si>
+  <si>
+    <t>Database/Availability/DemandOrder.csv</t>
+  </si>
+  <si>
+    <t>Database/Availability/SupplyOrder.csv</t>
+  </si>
+  <si>
+    <t>Database/Availability/BlockOrder.csv</t>
+  </si>
+  <si>
+    <t>Database/Price/DemandOrder.csv</t>
+  </si>
+  <si>
+    <t>Database/Price/SupplyOrder.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For datasets which have one file per country, replace the zone name (2 characters) in the path by ##. </t>
+  </si>
+  <si>
+    <t>Z2</t>
   </si>
 </sst>
 </file>
@@ -625,7 +601,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -685,15 +661,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
@@ -711,6 +678,16 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1053,8 +1030,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="C71" sqref="C71"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E144" sqref="E144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1071,16 +1048,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
-        <v>137</v>
-      </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
+      <c r="A1" s="26" t="s">
+        <v>130</v>
+      </c>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
     </row>
     <row r="2" spans="1:8" ht="3" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
@@ -1094,15 +1071,15 @@
     </row>
     <row r="3" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="28" t="s">
-        <v>138</v>
-      </c>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
+      <c r="B4" s="25" t="s">
+        <v>131</v>
+      </c>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
     </row>
     <row r="5" spans="1:8" s="8" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7"/>
@@ -1118,15 +1095,15 @@
       <c r="A6" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="27" t="s">
-        <v>139</v>
-      </c>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="27"/>
+      <c r="B6" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
     </row>
     <row r="7" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="12"/>
@@ -1158,11 +1135,11 @@
         <v>35</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="D18" s="13"/>
       <c r="H18" s="1" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
@@ -1209,25 +1186,25 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="19" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1251,7 +1228,7 @@
         <v>42370</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
@@ -1265,7 +1242,7 @@
         <v>42735</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
@@ -1279,7 +1256,7 @@
         <v>3</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
@@ -1317,7 +1294,7 @@
         <v>50</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="H47" s="1" t="s">
         <v>54</v>
@@ -1330,8 +1307,8 @@
       <c r="B48" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C48" s="26" t="s">
-        <v>147</v>
+      <c r="C48" s="23" t="s">
+        <v>139</v>
       </c>
       <c r="H48" s="1" t="s">
         <v>55</v>
@@ -1363,12 +1340,14 @@
         <v>35</v>
       </c>
       <c r="C62" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D62" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="H62" s="11"/>
+        <v>72</v>
+      </c>
+      <c r="H62" s="11" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
@@ -1377,145 +1356,139 @@
       <c r="B63" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C63" s="24" t="s">
-        <v>154</v>
+      <c r="C63" s="21" t="s">
+        <v>153</v>
       </c>
       <c r="D63" s="19" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="H63" s="11" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C64" s="20" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D64" s="19" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="H64" s="11" t="s">
-        <v>145</v>
+        <v>157</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C65" s="20" t="s">
-        <v>160</v>
-      </c>
+        <v>151</v>
+      </c>
+      <c r="C65" s="1"/>
       <c r="D65" s="19" t="s">
-        <v>78</v>
+        <v>72</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F65" s="5">
+        <v>1</v>
+      </c>
+      <c r="H65" s="11" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C66" s="20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D66" s="19" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="H66" s="11" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C67" s="20" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D67" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="H67" s="11" t="s">
-        <v>46</v>
+        <v>72</v>
+      </c>
+      <c r="H67" s="1" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C68" s="20" t="s">
-        <v>158</v>
-      </c>
+        <v>135</v>
+      </c>
+      <c r="C68" s="1"/>
       <c r="D68" s="19" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F68" s="5">
-        <v>50</v>
-      </c>
-      <c r="H68" s="11" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C69" s="20" t="s">
-        <v>162</v>
-      </c>
+        <v>143</v>
+      </c>
+      <c r="C69" s="1"/>
       <c r="D69" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="H69" s="1" t="s">
-        <v>48</v>
+        <v>72</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F69" s="5">
+        <v>50</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
-        <v>163</v>
+        <v>144</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C70" s="20" t="s">
-        <v>165</v>
+        <v>146</v>
       </c>
       <c r="D70" s="19"/>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
-        <v>164</v>
+        <v>145</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C71" s="20" t="s">
-        <v>166</v>
+        <v>147</v>
       </c>
       <c r="D71" s="19" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="72" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -1527,7 +1500,7 @@
       </c>
       <c r="C72" s="20"/>
       <c r="D72" s="19" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E72" s="1" t="s">
         <v>0</v>
@@ -1536,7 +1509,7 @@
         <v>20</v>
       </c>
       <c r="H72" s="1" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="73" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -1548,7 +1521,7 @@
       </c>
       <c r="C73" s="20"/>
       <c r="D73" s="19" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>0</v>
@@ -1559,14 +1532,14 @@
     </row>
     <row r="74" spans="1:8" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C74" s="20"/>
       <c r="D74" s="19" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E74" s="1" t="s">
         <v>0</v>
@@ -1577,14 +1550,14 @@
     </row>
     <row r="75" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C75" s="20"/>
       <c r="D75" s="19" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>0</v>
@@ -1595,26 +1568,26 @@
     </row>
     <row r="76" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C76" s="20"/>
       <c r="D76" s="19" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="77" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C77" s="20"/>
       <c r="D77" s="19" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>0</v>
@@ -1625,14 +1598,14 @@
     </row>
     <row r="78" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C78" s="20"/>
       <c r="D78" s="19" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E78" s="1" t="s">
         <v>0</v>
@@ -1643,26 +1616,26 @@
     </row>
     <row r="79" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C79" s="20"/>
       <c r="D79" s="19" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="80" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C80" s="20"/>
       <c r="D80" s="19" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E80" s="1" t="s">
         <v>0</v>
@@ -1673,14 +1646,14 @@
     </row>
     <row r="81" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C81" s="20"/>
       <c r="D81" s="19" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E81" s="1" t="s">
         <v>0</v>
@@ -1698,31 +1671,31 @@
     </row>
     <row r="86" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="87" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="25" t="s">
-        <v>146</v>
+      <c r="A87" s="22" t="s">
+        <v>138</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="C87" s="4" t="b">
         <v>1</v>
       </c>
       <c r="E87" s="6" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="F87" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="88" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="28" t="s">
+      <c r="A88" s="25" t="s">
         <v>45</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>129</v>
+        <v>158</v>
       </c>
       <c r="C88" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E88" s="6" t="s">
         <v>16</v>
@@ -1732,7 +1705,7 @@
       </c>
     </row>
     <row r="89" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="28"/>
+      <c r="A89" s="25"/>
       <c r="B89" s="6" t="s">
         <v>20</v>
       </c>
@@ -1747,9 +1720,9 @@
       </c>
     </row>
     <row r="90" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="28"/>
+      <c r="A90" s="25"/>
       <c r="B90" s="6" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="C90" s="4" t="b">
         <v>0</v>
@@ -1762,22 +1735,22 @@
       </c>
     </row>
     <row r="91" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="28"/>
+      <c r="A91" s="25"/>
       <c r="B91" s="6" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="C91" s="4" t="b">
         <v>0</v>
       </c>
       <c r="E91" s="6" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="F91" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="92" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="28"/>
+      <c r="A92" s="25"/>
       <c r="B92" s="6" t="s">
         <v>3</v>
       </c>
@@ -1785,29 +1758,29 @@
         <v>0</v>
       </c>
       <c r="E92" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="F92" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="25"/>
+      <c r="B93" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="F92" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="28"/>
-      <c r="B93" s="6" t="s">
-        <v>133</v>
-      </c>
       <c r="C93" s="4" t="b">
         <v>0</v>
       </c>
       <c r="E93" s="6" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="F93" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="94" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="28"/>
+      <c r="A94" s="25"/>
       <c r="B94" s="6" t="s">
         <v>29</v>
       </c>
@@ -1822,7 +1795,7 @@
       </c>
     </row>
     <row r="95" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="28"/>
+      <c r="A95" s="25"/>
       <c r="B95" s="6" t="s">
         <v>14</v>
       </c>
@@ -1830,14 +1803,14 @@
         <v>0</v>
       </c>
       <c r="E95" s="6" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="F95" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="96" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A96" s="28"/>
+      <c r="A96" s="25"/>
       <c r="B96" s="6" t="s">
         <v>4</v>
       </c>
@@ -1852,7 +1825,7 @@
       </c>
     </row>
     <row r="97" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="28"/>
+      <c r="A97" s="25"/>
       <c r="B97" s="6" t="s">
         <v>6</v>
       </c>
@@ -1867,7 +1840,7 @@
       </c>
     </row>
     <row r="98" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="28"/>
+      <c r="A98" s="25"/>
       <c r="B98" s="6" t="s">
         <v>5</v>
       </c>
@@ -1882,7 +1855,7 @@
       </c>
     </row>
     <row r="99" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="28"/>
+      <c r="A99" s="25"/>
       <c r="B99" s="6" t="s">
         <v>7</v>
       </c>
@@ -1897,7 +1870,7 @@
       </c>
     </row>
     <row r="100" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="28"/>
+      <c r="A100" s="25"/>
       <c r="B100" s="6" t="s">
         <v>9</v>
       </c>
@@ -1905,14 +1878,14 @@
         <v>0</v>
       </c>
       <c r="E100" s="6" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="F100" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="101" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="28"/>
+      <c r="A101" s="25"/>
       <c r="B101" s="6" t="s">
         <v>10</v>
       </c>
@@ -1920,14 +1893,14 @@
         <v>0</v>
       </c>
       <c r="E101" s="6" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="F101" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="102" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="28"/>
+      <c r="A102" s="25"/>
       <c r="B102" s="6" t="s">
         <v>26</v>
       </c>
@@ -1977,7 +1950,7 @@
         <v>0</v>
       </c>
       <c r="E105" s="6" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="F105" s="4" t="b">
         <v>0</v>
@@ -1991,10 +1964,10 @@
         <v>0</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="E106" s="6" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="F106" s="4" t="b">
         <v>0</v>
@@ -2002,7 +1975,7 @@
     </row>
     <row r="107" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B107" s="6" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="C107" s="4" t="b">
         <v>0</v>
@@ -2014,7 +1987,7 @@
         <v>0</v>
       </c>
       <c r="H107" s="1" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
     </row>
     <row r="108" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -2025,7 +1998,7 @@
         <v>0</v>
       </c>
       <c r="E108" s="6" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="F108" s="4" t="b">
         <v>0</v>
@@ -2037,7 +2010,7 @@
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.3">
@@ -2045,7 +2018,7 @@
         <v>1</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C112" s="5">
         <v>1</v>
@@ -2053,38 +2026,38 @@
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C113" s="5">
         <v>1</v>
       </c>
       <c r="H113" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B114" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B114" s="1" t="s">
-        <v>65</v>
-      </c>
       <c r="C114" s="5">
         <v>1</v>
       </c>
       <c r="H114" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C115" s="5">
         <v>1</v>
@@ -2108,126 +2081,126 @@
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130" s="2" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B132" s="23" t="s">
+      <c r="B132" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="C132" s="28" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B133" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="C133" s="28" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B134" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="C134" s="28" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B135" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="C135" s="28" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B136" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="C136" s="28" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B137" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="C137" s="28" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B138" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="C132" s="22" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B133" s="23" t="s">
+      <c r="C138" s="28" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B139" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="C133" s="22" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B134" s="23" t="s">
+      <c r="C139" s="28" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B140" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="C134" s="22" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B135" s="23" t="s">
+      <c r="C140" s="28" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B141" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="C135" s="22" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B136" s="23" t="s">
+      <c r="C141" s="28" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B142" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="C136" s="22" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B137" s="23" t="s">
+      <c r="C142" s="28" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B143" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="C137" s="22" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B138" s="23" t="s">
+      <c r="C143" s="28" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B144" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="C138" s="22" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B139" s="23" t="s">
+      <c r="C144" s="28" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B145" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="C139" s="22" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B140" s="23" t="s">
+      <c r="C145" s="28" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B146" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="C140" s="22" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B141" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="C141" s="22" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B142" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="C142" s="22" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B143" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="C143" s="22" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B144" s="23" t="s">
-        <v>91</v>
-      </c>
-      <c r="C144" s="22" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="145" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B145" s="23" t="s">
-        <v>92</v>
-      </c>
-      <c r="C145" s="22" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="146" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B146" s="23" t="s">
-        <v>93</v>
-      </c>
-      <c r="C146" s="22" t="b">
+      <c r="C146" s="28" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2260,7 +2233,7 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Multiplicative Factor" prompt="This modifier multiplies the PV generation curves of all the zones by the provided factor" sqref="C114" xr:uid="{00000000-0002-0000-0000-000007000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Multiplicative Factor" prompt="This modifier multiplies the storage capacity in all the zones by the provided factor" sqref="C115" xr:uid="{00000000-0002-0000-0000-000008000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to the gams folder" prompt="Example:_x000a_C:\GAMS\win64\24.3_x000a__x000a_If unspecified or non-existing, Dispa-SET will try to determine the path automatically. " sqref="C22" xr:uid="{00000000-0002-0000-0000-000009000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default value (% of max load)" prompt="In case no data file is provided. This single value is used for all the sets._x000a_It is defined in % of the maximum load throughout the simulation period." sqref="F68" xr:uid="{56B7C1C7-C83A-40F5-A03D-AFAA1755A969}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default value (% of max load)" prompt="In case no data file is provided. This single value is used for all the sets._x000a_It is defined in % of the maximum load throughout the simulation period." sqref="F68:F69 F65" xr:uid="{56B7C1C7-C83A-40F5-A03D-AFAA1755A969}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default value (in EUR/t_co2)" prompt="In case no data file is provided. This single value is used for all the sets." sqref="F75" xr:uid="{00000000-0002-0000-0000-00000B000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to the cplex executable" prompt="This is only useful if the Pyomo engine is selected and if cplex is not in the PATH (i.e. accessible from the prompt). This parameters can be left unspecified in most cases._x000a__x000a_Example:_x000a_C:\\Users\\ese-veda06\\Downloads\\solvers\\cplex.exe" sqref="C23" xr:uid="{00000000-0002-0000-0000-00000C000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path the outage data" prompt="Select the path the outage csv file from the database._x000a__x000a_The path should be relative to this excel file. Use &quot;..&quot; to go up one folder. Folder separator can be either &quot;/&quot; or &quot;\&quot;" sqref="C63" xr:uid="{00000000-0002-0000-0000-00000E000000}"/>
@@ -2323,10 +2296,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2334,10 +2307,9 @@
     <col min="1" max="1" width="23.6640625" customWidth="1"/>
     <col min="2" max="2" width="32.5546875" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="4" max="4" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
         <v>2</v>
       </c>
@@ -2347,40 +2319,21 @@
       <c r="C1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="17" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="b">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="C2" t="s">
-        <v>147</v>
-      </c>
-      <c r="D2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="b">
         <v>0</v>
-      </c>
-      <c r="D3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="D4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="D5" t="s">
-        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -2395,7 +2348,7 @@
   <dimension ref="A1:O16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:XFD23"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2404,751 +2357,752 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="17" t="s">
+      <c r="A1" s="29"/>
+      <c r="B1" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="C1" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="D1" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="E1" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="F1" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="G1" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="H1" s="29" t="s">
         <v>94</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="I1" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="J1" s="29" t="s">
         <v>96</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="K1" s="29" t="s">
         <v>97</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="L1" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="M1" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="N1" s="29" t="s">
         <v>100</v>
       </c>
-      <c r="I1" s="17" t="s">
+      <c r="O1" s="29" t="s">
         <v>101</v>
       </c>
-      <c r="J1" s="17" t="s">
-        <v>102</v>
-      </c>
-      <c r="K1" s="17" t="s">
-        <v>103</v>
-      </c>
-      <c r="L1" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="M1" s="17" t="s">
-        <v>105</v>
-      </c>
-      <c r="N1" s="17" t="s">
-        <v>106</v>
-      </c>
-      <c r="O1" s="17" t="s">
-        <v>107</v>
-      </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="C2" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="E2" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="F2" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="G2" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="H2" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="I2" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="J2" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="K2" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="L2" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="M2" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="N2" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="O2" s="30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="C3" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="G3" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="H3" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="I3" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="J3" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="K3" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="L3" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="M3" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="N3" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="O3" s="30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="C4" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="E4" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="F4" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="G4" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="I4" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="J4" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="K4" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="L4" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="M4" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="N4" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="O4" s="30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="F5" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="I5" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="J5" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="K5" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="L5" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="M5" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="N5" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="O5" s="30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A6" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="B6" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="C6" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="D6" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="F6" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="H6" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="I6" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="J6" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="K6" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="L6" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="M6" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="N6" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="O6" s="30" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A7" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="B7" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="C7" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="D7" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="E7" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="F7" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="G7" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="H7" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="I7" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="J7" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="K7" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="L7" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="M7" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="N7" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="O7" s="30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A8" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="B2" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="C2" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="D2" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="E2" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="F2" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="G2" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="H2" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="I2" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="J2" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="K2" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="L2" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="M2" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="N2" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="O2" s="21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" s="17" t="s">
+      <c r="B8" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="C8" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="E8" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="F8" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="G8" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="H8" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="I8" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="J8" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="K8" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="L8" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="M8" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="N8" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="O8" s="30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A9" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="B3" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="C3" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="D3" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="E3" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="F3" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="G3" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="H3" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="I3" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="J3" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="K3" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="L3" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="M3" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="N3" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="O3" s="21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" s="17" t="s">
+      <c r="B9" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="C9" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="D9" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="E9" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="F9" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="G9" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="H9" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="I9" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="J9" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="K9" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="L9" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="M9" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="N9" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="O9" s="30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A10" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="B4" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="C4" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="D4" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="E4" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="F4" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="G4" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="H4" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="I4" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="J4" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="K4" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="L4" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="M4" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="N4" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="O4" s="21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A5" s="17" t="s">
+      <c r="B10" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="C10" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D10" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="E10" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="F10" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="G10" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="H10" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="I10" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="J10" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="K10" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="L10" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="M10" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="N10" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="O10" s="30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A11" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="B5" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="C5" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="D5" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="E5" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="F5" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="G5" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="H5" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="I5" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="J5" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="K5" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="L5" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="M5" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="N5" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="O5" s="21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" s="17" t="s">
+      <c r="B11" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="C11" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D11" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="E11" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="F11" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="G11" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="H11" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="I11" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="J11" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="K11" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="L11" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="M11" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="N11" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="O11" s="30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A12" s="29" t="s">
         <v>83</v>
       </c>
-      <c r="B6" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="C6" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="D6" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="E6" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="F6" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="G6" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="H6" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="I6" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="J6" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="K6" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="L6" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="M6" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="N6" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="O6" s="21" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" s="17" t="s">
+      <c r="B12" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="C12" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="D12" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="E12" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="F12" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="G12" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="H12" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="I12" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="J12" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="K12" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="L12" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="M12" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="N12" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="O12" s="30" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A13" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="B7" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="C7" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="D7" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="E7" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="F7" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="G7" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="H7" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="I7" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="J7" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="K7" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="L7" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="M7" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="N7" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="O7" s="21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" s="17" t="s">
+      <c r="B13" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="C13" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="D13" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="E13" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="F13" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="G13" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="H13" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="I13" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="J13" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="K13" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="L13" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="M13" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="N13" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="O13" s="30" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A14" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="B8" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="C8" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="D8" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="E8" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="F8" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="G8" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="H8" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="I8" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="J8" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="K8" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="L8" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="M8" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="N8" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="O8" s="21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A9" s="17" t="s">
+      <c r="B14" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="C14" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="D14" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="E14" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="F14" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="G14" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="H14" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="I14" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="J14" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="K14" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="L14" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="M14" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="N14" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="O14" s="30" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A15" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="B9" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="C9" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="D9" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="E9" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="F9" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="G9" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="H9" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="I9" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="J9" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="K9" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="L9" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="M9" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="N9" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="O9" s="21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" s="17" t="s">
+      <c r="B15" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="C15" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D15" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="E15" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="F15" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="G15" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="H15" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="I15" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="J15" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="K15" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="L15" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="M15" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="N15" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="O15" s="30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A16" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="B10" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="C10" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="D10" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="E10" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="F10" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="G10" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="H10" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="I10" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="J10" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="K10" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="L10" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="M10" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="N10" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="O10" s="21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="B11" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="C11" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="D11" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="E11" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="F11" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="G11" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="H11" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="I11" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="J11" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="K11" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="L11" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="M11" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="N11" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="O11" s="21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A12" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="B12" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="C12" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="D12" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="E12" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="F12" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="G12" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="H12" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="I12" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="J12" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="K12" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="L12" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="M12" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="N12" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="O12" s="21" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A13" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="B13" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="C13" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="D13" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="E13" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="F13" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="G13" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="H13" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="I13" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="J13" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="K13" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="L13" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="M13" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="N13" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="O13" s="21" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A14" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="B14" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="C14" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="D14" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="E14" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="F14" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="G14" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="H14" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="I14" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="J14" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="K14" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="L14" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="M14" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="N14" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="O14" s="21" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A15" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="B15" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="C15" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="D15" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="E15" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="F15" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="G15" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="H15" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="I15" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="J15" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="K15" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="L15" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="M15" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="N15" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="O15" s="21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A16" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="B16" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="C16" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="D16" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="E16" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="F16" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="G16" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="H16" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="I16" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="J16" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="K16" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="L16" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="M16" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="N16" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="O16" s="21" t="b">
+      <c r="B16" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="C16" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D16" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="E16" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="F16" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="G16" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="H16" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="I16" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="J16" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="K16" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="L16" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="M16" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="N16" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="O16" s="30" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Populated database and data preprocessing
</commit_message>
<xml_diff>
--- a/ConfigFiles/ConfigTest.xlsx
+++ b/ConfigFiles/ConfigTest.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22130"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matij\Documents\Github\Heating\Heat-Markets\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB5EF2D9-D2B5-40B9-B4D1-44FE9BE70A3F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00B62829-9131-4F4A-804F-A3572C1CEB2D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="153">
   <si>
     <t>Default value</t>
   </si>
@@ -173,9 +173,6 @@
     <t xml:space="preserve">for example: </t>
   </si>
   <si>
-    <t>../data/Demand/##/2014/load.csv</t>
-  </si>
-  <si>
     <t>will fetch one load.csv file per country, by replacing ## with FR, DE, NL, etc.</t>
   </si>
   <si>
@@ -188,12 +185,6 @@
     <t>Reserve calculation</t>
   </si>
   <si>
-    <t>Price of Gas</t>
-  </si>
-  <si>
-    <t>Price of Fuel-Oil</t>
-  </si>
-  <si>
     <t>This sections defines parameters that influence the formulation of the problem</t>
   </si>
   <si>
@@ -341,30 +332,9 @@
     <t>Participation to reserve markets</t>
   </si>
   <si>
-    <t>Price of Biomass</t>
-  </si>
-  <si>
-    <t>Price of CO2</t>
-  </si>
-  <si>
-    <t>All fuel prices are in EUR/MWh of primary energy (lower heating value)</t>
-  </si>
-  <si>
-    <t>Reservoir Levels</t>
-  </si>
-  <si>
-    <t>Price of Lignite</t>
-  </si>
-  <si>
-    <t>Price of Peat</t>
-  </si>
-  <si>
     <t>CPLEX path</t>
   </si>
   <si>
-    <t>Heat Demand</t>
-  </si>
-  <si>
     <t>BE</t>
   </si>
   <si>
@@ -374,12 +344,6 @@
     <t>Standard</t>
   </si>
   <si>
-    <t>Price of unserved heat</t>
-  </si>
-  <si>
-    <t>Load Shedding Cost</t>
-  </si>
-  <si>
     <t xml:space="preserve">NB: Ireland (IE) includes north Ireland. </t>
   </si>
   <si>
@@ -488,25 +452,43 @@
     <t>Availability - Flexible Order</t>
   </si>
   <si>
-    <t>Database/Availability/DemandOrder.csv</t>
-  </si>
-  <si>
-    <t>Database/Availability/SupplyOrder.csv</t>
-  </si>
-  <si>
-    <t>Database/Availability/BlockOrder.csv</t>
-  </si>
-  <si>
-    <t>Database/Price/DemandOrder.csv</t>
-  </si>
-  <si>
-    <t>Database/Price/SupplyOrder.csv</t>
-  </si>
-  <si>
     <t xml:space="preserve">For datasets which have one file per country, replace the zone name (2 characters) in the path by ##. </t>
   </si>
   <si>
     <t>Z2</t>
+  </si>
+  <si>
+    <t>Database/Availability/##/DemandOrder.csv</t>
+  </si>
+  <si>
+    <t>Database/Availability/##/BlockOrder.csv</t>
+  </si>
+  <si>
+    <t>Database/Availability/##/SimpleOrder.csv</t>
+  </si>
+  <si>
+    <t>..Database/Availability/##/DemandOrder.csv</t>
+  </si>
+  <si>
+    <t>Interconnections</t>
+  </si>
+  <si>
+    <t>EUR/MWh</t>
+  </si>
+  <si>
+    <t>Database/Interconnections/NTC/NTC.csv</t>
+  </si>
+  <si>
+    <t>NTC</t>
+  </si>
+  <si>
+    <t>Database/Interconnections/CBF/CBF.csv</t>
+  </si>
+  <si>
+    <t>Database/Price/##/PriceDemandOrder.csv</t>
+  </si>
+  <si>
+    <t>Database/Price/##/PriceSimpleOrder.csv</t>
   </si>
 </sst>
 </file>
@@ -670,15 +652,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -688,6 +661,15 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1030,8 +1012,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H165"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E144" sqref="E144"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="C68" sqref="C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1048,16 +1030,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
-        <v>130</v>
-      </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
+      <c r="A1" s="30" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
     </row>
     <row r="2" spans="1:8" ht="3" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
@@ -1071,15 +1053,15 @@
     </row>
     <row r="3" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="25" t="s">
-        <v>131</v>
-      </c>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25"/>
+      <c r="B4" s="29" t="s">
+        <v>119</v>
+      </c>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
     </row>
     <row r="5" spans="1:8" s="8" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7"/>
@@ -1095,15 +1077,15 @@
       <c r="A6" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
+      <c r="B6" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
     </row>
     <row r="7" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="12"/>
@@ -1135,11 +1117,11 @@
         <v>35</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="D18" s="13"/>
       <c r="H18" s="1" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
@@ -1153,7 +1135,7 @@
         <v>0</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
@@ -1167,7 +1149,7 @@
         <v>1</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
@@ -1181,30 +1163,30 @@
         <v>1</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="19" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1228,7 +1210,7 @@
         <v>42370</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
@@ -1239,10 +1221,10 @@
         <v>36</v>
       </c>
       <c r="C32" s="18">
-        <v>42735</v>
+        <v>42371</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
@@ -1253,10 +1235,10 @@
         <v>42</v>
       </c>
       <c r="C33" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
@@ -1291,27 +1273,27 @@
         <v>39</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C48" s="23" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="9" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1334,62 +1316,62 @@
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C62" s="20" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="D62" s="19" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="H62" s="11" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C63" s="21" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="D63" s="19" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="H63" s="11" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C64" s="20" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="D64" s="19" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="H64" s="11" t="s">
-        <v>157</v>
+        <v>140</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="C65" s="1"/>
       <c r="D65" s="19" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>0</v>
@@ -1403,45 +1385,45 @@
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C66" s="20" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D66" s="19" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="H66" s="11" t="s">
-        <v>47</v>
+        <v>145</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C67" s="20" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D67" s="19" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="C68" s="1"/>
       <c r="D68" s="19" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>0</v>
@@ -1449,14 +1431,17 @@
       <c r="F68" s="5">
         <v>30</v>
       </c>
+      <c r="H68" s="1" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="C69" s="1"/>
       <c r="D69" s="19" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>0</v>
@@ -1464,207 +1449,72 @@
       <c r="F69" s="5">
         <v>50</v>
       </c>
+      <c r="H69" s="1" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C70" s="20" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="D70" s="19"/>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C71" s="20" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="D71" s="19" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
-        <v>52</v>
+        <v>146</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C72" s="20"/>
+      <c r="C72" s="20" t="s">
+        <v>150</v>
+      </c>
       <c r="D72" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="E72" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F72" s="5">
-        <v>20</v>
-      </c>
-      <c r="H72" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
-        <v>53</v>
+        <v>149</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C73" s="20"/>
-      <c r="D73" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="E73" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F73" s="5">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C74" s="20"/>
-      <c r="D74" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="E74" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F74" s="5">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C75" s="20"/>
-      <c r="D75" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="E75" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F75" s="5">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C76" s="20"/>
-      <c r="D76" s="19" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C77" s="20"/>
-      <c r="D77" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="E77" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F77" s="5">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C78" s="20"/>
-      <c r="D78" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="E78" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F78" s="5">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C79" s="20"/>
-      <c r="D79" s="19" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="B80" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C80" s="20"/>
-      <c r="D80" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="E80" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F80" s="5">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C81" s="20"/>
-      <c r="D81" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="E81" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F81" s="5">
-        <v>400</v>
-      </c>
-    </row>
+      <c r="C73" s="20" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="75" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="76" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="77" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="78" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="79" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="80" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="81" spans="1:6" hidden="1" x14ac:dyDescent="0.3"/>
     <row r="82" spans="1:6" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="83" spans="1:6" ht="4.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="84" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="83" spans="1:6" ht="4.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="84" spans="1:6" ht="9" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="85" spans="1:6" s="10" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="9"/>
       <c r="C85" s="15"/>
@@ -1672,27 +1522,27 @@
     <row r="86" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="87" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="22" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="C87" s="4" t="b">
         <v>1</v>
       </c>
       <c r="E87" s="6" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="F87" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="88" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="25" t="s">
+      <c r="A88" s="29" t="s">
         <v>45</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>158</v>
+        <v>141</v>
       </c>
       <c r="C88" s="4" t="b">
         <v>1</v>
@@ -1705,7 +1555,7 @@
       </c>
     </row>
     <row r="89" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="25"/>
+      <c r="A89" s="29"/>
       <c r="B89" s="6" t="s">
         <v>20</v>
       </c>
@@ -1720,9 +1570,9 @@
       </c>
     </row>
     <row r="90" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="25"/>
+      <c r="A90" s="29"/>
       <c r="B90" s="6" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="C90" s="4" t="b">
         <v>0</v>
@@ -1735,22 +1585,22 @@
       </c>
     </row>
     <row r="91" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="25"/>
+      <c r="A91" s="29"/>
       <c r="B91" s="6" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="C91" s="4" t="b">
         <v>0</v>
       </c>
       <c r="E91" s="6" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="F91" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="92" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="25"/>
+      <c r="A92" s="29"/>
       <c r="B92" s="6" t="s">
         <v>3</v>
       </c>
@@ -1758,29 +1608,29 @@
         <v>0</v>
       </c>
       <c r="E92" s="6" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="F92" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="93" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="25"/>
+      <c r="A93" s="29"/>
       <c r="B93" s="6" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="C93" s="4" t="b">
         <v>0</v>
       </c>
       <c r="E93" s="6" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="F93" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="94" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="25"/>
+      <c r="A94" s="29"/>
       <c r="B94" s="6" t="s">
         <v>29</v>
       </c>
@@ -1795,7 +1645,7 @@
       </c>
     </row>
     <row r="95" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="25"/>
+      <c r="A95" s="29"/>
       <c r="B95" s="6" t="s">
         <v>14</v>
       </c>
@@ -1803,14 +1653,14 @@
         <v>0</v>
       </c>
       <c r="E95" s="6" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="F95" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="96" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A96" s="25"/>
+      <c r="A96" s="29"/>
       <c r="B96" s="6" t="s">
         <v>4</v>
       </c>
@@ -1825,7 +1675,7 @@
       </c>
     </row>
     <row r="97" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="25"/>
+      <c r="A97" s="29"/>
       <c r="B97" s="6" t="s">
         <v>6</v>
       </c>
@@ -1840,7 +1690,7 @@
       </c>
     </row>
     <row r="98" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="25"/>
+      <c r="A98" s="29"/>
       <c r="B98" s="6" t="s">
         <v>5</v>
       </c>
@@ -1855,7 +1705,7 @@
       </c>
     </row>
     <row r="99" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="25"/>
+      <c r="A99" s="29"/>
       <c r="B99" s="6" t="s">
         <v>7</v>
       </c>
@@ -1870,7 +1720,7 @@
       </c>
     </row>
     <row r="100" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="25"/>
+      <c r="A100" s="29"/>
       <c r="B100" s="6" t="s">
         <v>9</v>
       </c>
@@ -1878,14 +1728,14 @@
         <v>0</v>
       </c>
       <c r="E100" s="6" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="F100" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="101" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="25"/>
+      <c r="A101" s="29"/>
       <c r="B101" s="6" t="s">
         <v>10</v>
       </c>
@@ -1893,14 +1743,14 @@
         <v>0</v>
       </c>
       <c r="E101" s="6" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="F101" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="102" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="25"/>
+      <c r="A102" s="29"/>
       <c r="B102" s="6" t="s">
         <v>26</v>
       </c>
@@ -1950,7 +1800,7 @@
         <v>0</v>
       </c>
       <c r="E105" s="6" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="F105" s="4" t="b">
         <v>0</v>
@@ -1964,10 +1814,10 @@
         <v>0</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="E106" s="6" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="F106" s="4" t="b">
         <v>0</v>
@@ -1975,7 +1825,7 @@
     </row>
     <row r="107" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B107" s="6" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="C107" s="4" t="b">
         <v>0</v>
@@ -1987,7 +1837,7 @@
         <v>0</v>
       </c>
       <c r="H107" s="1" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
     </row>
     <row r="108" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -1998,7 +1848,7 @@
         <v>0</v>
       </c>
       <c r="E108" s="6" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="F108" s="4" t="b">
         <v>0</v>
@@ -2010,7 +1860,7 @@
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.3">
@@ -2018,7 +1868,7 @@
         <v>1</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C112" s="5">
         <v>1</v>
@@ -2026,38 +1876,38 @@
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C113" s="5">
         <v>1</v>
       </c>
       <c r="H113" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B114" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C114" s="5">
+        <v>1</v>
+      </c>
+      <c r="H114" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="C114" s="5">
-        <v>1</v>
-      </c>
-      <c r="H114" s="1" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C115" s="5">
         <v>1</v>
@@ -2081,126 +1931,126 @@
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B132" s="27" t="s">
+      <c r="B132" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="C132" s="25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B133" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="C133" s="25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B134" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="C134" s="25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B135" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="C132" s="28" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B133" s="27" t="s">
+      <c r="C135" s="25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B136" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="C133" s="28" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B134" s="27" t="s">
+      <c r="C136" s="25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B137" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="C134" s="28" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B135" s="27" t="s">
+      <c r="C137" s="25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B138" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="C135" s="28" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B136" s="27" t="s">
+      <c r="C138" s="25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B139" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="C136" s="28" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B137" s="27" t="s">
+      <c r="C139" s="25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B140" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="C137" s="28" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B138" s="27" t="s">
+      <c r="C140" s="25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B141" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="C138" s="28" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B139" s="27" t="s">
+      <c r="C141" s="25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B142" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="C139" s="28" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B140" s="27" t="s">
+      <c r="C142" s="25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B143" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="C140" s="28" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B141" s="27" t="s">
+      <c r="C143" s="25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B144" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="C141" s="28" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B142" s="27" t="s">
+      <c r="C144" s="25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B145" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="C142" s="28" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B143" s="27" t="s">
+      <c r="C145" s="25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B146" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="C143" s="28" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B144" s="27" t="s">
-        <v>85</v>
-      </c>
-      <c r="C144" s="28" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="145" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B145" s="27" t="s">
-        <v>86</v>
-      </c>
-      <c r="C145" s="28" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="146" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B146" s="27" t="s">
-        <v>87</v>
-      </c>
-      <c r="C146" s="28" t="b">
+      <c r="C146" s="25" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2217,7 +2067,7 @@
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="B4:H4"/>
   </mergeCells>
-  <dataValidations count="15">
+  <dataValidations count="13">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path the simulation directory" prompt="All inputs are saved in the so-called simulation directory, which includes, excel , gdx and pickle files together with the GAMS files._x000a__x000a_The path should be relative to this excel file. Use &quot;..&quot; to go up one folder. Folder separator can be either &quot;/&quot; or &quot;\&quot;" sqref="C18:D18" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
     <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Start day of the simulation" prompt="This is the simulated day. It must be comprised within the range of dates provided within the data files." sqref="C31" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>1</formula1>
@@ -2227,14 +2077,12 @@
       <formula1>1</formula1>
       <formula2>73051</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default value" prompt="In case no data file is provided. This single value is used for all the sets." sqref="F80:F81 F77:F78 F72:F74" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Multiplicative Factor" prompt="This modifier multiplies the demand curves of all the zones by the provided factor" sqref="C112" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Multiplicative Factor" prompt="This modifier multiplies the wind generation curves of all the zones by the provided factor" sqref="C113" xr:uid="{00000000-0002-0000-0000-000006000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Multiplicative Factor" prompt="This modifier multiplies the PV generation curves of all the zones by the provided factor" sqref="C114" xr:uid="{00000000-0002-0000-0000-000007000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Multiplicative Factor" prompt="This modifier multiplies the storage capacity in all the zones by the provided factor" sqref="C115" xr:uid="{00000000-0002-0000-0000-000008000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to the gams folder" prompt="Example:_x000a_C:\GAMS\win64\24.3_x000a__x000a_If unspecified or non-existing, Dispa-SET will try to determine the path automatically. " sqref="C22" xr:uid="{00000000-0002-0000-0000-000009000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default value (% of max load)" prompt="In case no data file is provided. This single value is used for all the sets._x000a_It is defined in % of the maximum load throughout the simulation period." sqref="F68:F69 F65" xr:uid="{56B7C1C7-C83A-40F5-A03D-AFAA1755A969}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default value (in EUR/t_co2)" prompt="In case no data file is provided. This single value is used for all the sets." sqref="F75" xr:uid="{00000000-0002-0000-0000-00000B000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to the cplex executable" prompt="This is only useful if the Pyomo engine is selected and if cplex is not in the PATH (i.e. accessible from the prompt). This parameters can be left unspecified in most cases._x000a__x000a_Example:_x000a_C:\\Users\\ese-veda06\\Downloads\\solvers\\cplex.exe" sqref="C23" xr:uid="{00000000-0002-0000-0000-00000C000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path the outage data" prompt="Select the path the outage csv file from the database._x000a__x000a_The path should be relative to this excel file. Use &quot;..&quot; to go up one folder. Folder separator can be either &quot;/&quot; or &quot;\&quot;" sqref="C63" xr:uid="{00000000-0002-0000-0000-00000E000000}"/>
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Look Ahead Period" prompt="This is the overlap period between consecutive optimization of the rolling horizon._x000a__x000a_If HorizonLength is 3 and  LookAhead is 1, optimization length is 4 days, discarding 1 day each time" sqref="C34" xr:uid="{00000000-0002-0000-0000-00000F000000}">
@@ -2317,7 +2165,7 @@
         <v>40</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -2325,10 +2173,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="C2" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -2357,752 +2205,752 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="29"/>
-      <c r="B1" s="29" t="s">
+      <c r="A1" s="26"/>
+      <c r="B1" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="E1" s="26" t="s">
         <v>88</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="F1" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="G1" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="H1" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="I1" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="G1" s="29" t="s">
+      <c r="J1" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="H1" s="29" t="s">
+      <c r="K1" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="I1" s="29" t="s">
+      <c r="L1" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="J1" s="29" t="s">
+      <c r="M1" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="K1" s="29" t="s">
+      <c r="N1" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="L1" s="29" t="s">
+      <c r="O1" s="26" t="s">
         <v>98</v>
       </c>
-      <c r="M1" s="29" t="s">
-        <v>99</v>
-      </c>
-      <c r="N1" s="29" t="s">
-        <v>100</v>
-      </c>
-      <c r="O1" s="29" t="s">
-        <v>101</v>
-      </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="C2" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="E2" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="F2" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="G2" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="H2" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="I2" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="J2" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="K2" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="L2" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="M2" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="N2" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="O2" s="27" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="C3" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="G3" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="H3" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="I3" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="J3" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="K3" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="L3" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="M3" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="N3" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="O3" s="27" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="C4" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="E4" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="F4" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="G4" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="I4" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="J4" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="K4" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="L4" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="M4" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="N4" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="O4" s="27" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="C2" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="D2" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="E2" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="F2" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="G2" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="H2" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="I2" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="J2" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="K2" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="L2" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="M2" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="N2" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="O2" s="30" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" s="29" t="s">
+      <c r="B5" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="F5" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="I5" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="J5" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="K5" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="L5" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="M5" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="N5" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="O5" s="27" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A6" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="B3" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="C3" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="D3" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="E3" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="F3" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="G3" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="H3" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="I3" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="J3" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="K3" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="L3" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="M3" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="N3" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="O3" s="30" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" s="29" t="s">
+      <c r="B6" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="C6" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="D6" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="F6" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="H6" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="I6" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="J6" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="K6" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="L6" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="M6" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="N6" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="O6" s="27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A7" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="B4" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="C4" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D4" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="E4" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="F4" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="G4" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="H4" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="I4" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="J4" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="K4" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="L4" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="M4" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="N4" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="O4" s="30" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A5" s="29" t="s">
+      <c r="B7" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="C7" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="D7" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="E7" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="F7" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="G7" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="H7" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="I7" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="J7" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="K7" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="L7" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="M7" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="N7" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="O7" s="27" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A8" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="B5" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="C5" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D5" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="E5" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="F5" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="G5" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="H5" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="I5" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="J5" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="K5" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="L5" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="M5" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="N5" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="O5" s="30" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" s="29" t="s">
+      <c r="B8" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="C8" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="E8" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="F8" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="G8" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="H8" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="I8" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="J8" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="K8" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="L8" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="M8" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="N8" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="O8" s="27" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A9" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="B6" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="C6" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="D6" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="E6" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="F6" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="G6" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="H6" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="I6" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="J6" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="K6" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="L6" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="M6" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="N6" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="O6" s="30" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" s="29" t="s">
+      <c r="B9" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="C9" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="D9" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="E9" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="F9" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="G9" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="H9" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="I9" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="J9" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="K9" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="L9" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="M9" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="N9" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="O9" s="27" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A10" s="26" t="s">
         <v>78</v>
       </c>
-      <c r="B7" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="C7" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="D7" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="E7" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="F7" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="G7" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="H7" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="I7" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="J7" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="K7" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="L7" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="M7" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="N7" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="O7" s="30" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" s="29" t="s">
+      <c r="B10" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="C10" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="D10" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="E10" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="F10" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="G10" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="H10" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="I10" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="J10" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="K10" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="L10" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="M10" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="N10" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="O10" s="27" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A11" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="B8" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="C8" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D8" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="E8" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="F8" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="G8" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="H8" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="I8" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="J8" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="K8" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="L8" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="M8" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="N8" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="O8" s="30" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A9" s="29" t="s">
+      <c r="B11" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="C11" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="D11" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="E11" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="F11" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="G11" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="H11" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="I11" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="J11" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="K11" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="L11" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="M11" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="N11" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="O11" s="27" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A12" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="B9" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="C9" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="D9" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="E9" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="F9" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="G9" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="H9" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="I9" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="J9" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="K9" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="L9" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="M9" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="N9" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="O9" s="30" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" s="29" t="s">
+      <c r="B12" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="C12" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="D12" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="E12" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="F12" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="G12" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="H12" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="I12" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="J12" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="K12" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="L12" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="M12" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="N12" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="O12" s="27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A13" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="B10" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="C10" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D10" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="E10" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="F10" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="G10" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="H10" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="I10" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="J10" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="K10" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="L10" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="M10" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="N10" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="O10" s="30" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" s="29" t="s">
+      <c r="B13" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="C13" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="D13" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="E13" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="F13" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="G13" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="H13" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="I13" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="J13" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="K13" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="L13" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="M13" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="N13" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="O13" s="27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A14" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="B11" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="C11" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D11" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="E11" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="F11" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="G11" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="H11" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="I11" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="J11" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="K11" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="L11" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="M11" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="N11" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="O11" s="30" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A12" s="29" t="s">
+      <c r="B14" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="C14" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="D14" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="E14" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="F14" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="G14" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="H14" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="I14" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="J14" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="K14" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="L14" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="M14" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="N14" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="O14" s="27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A15" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="B12" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="C12" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="D12" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="E12" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="F12" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="G12" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="H12" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="I12" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="J12" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="K12" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="L12" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="M12" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="N12" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="O12" s="30" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A13" s="29" t="s">
+      <c r="B15" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="C15" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="D15" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="E15" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="F15" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="G15" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="H15" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="I15" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="J15" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="K15" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="L15" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="M15" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="N15" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="O15" s="27" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A16" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="B13" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="C13" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="D13" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="E13" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="F13" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="G13" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="H13" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="I13" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="J13" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="K13" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="L13" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="M13" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="N13" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="O13" s="30" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A14" s="29" t="s">
-        <v>85</v>
-      </c>
-      <c r="B14" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="C14" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="D14" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="E14" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="F14" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="G14" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="H14" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="I14" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="J14" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="K14" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="L14" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="M14" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="N14" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="O14" s="30" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A15" s="29" t="s">
-        <v>86</v>
-      </c>
-      <c r="B15" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="C15" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D15" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="E15" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="F15" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="G15" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="H15" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="I15" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="J15" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="K15" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="L15" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="M15" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="N15" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="O15" s="30" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A16" s="29" t="s">
-        <v>87</v>
-      </c>
-      <c r="B16" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="C16" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D16" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="E16" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="F16" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="G16" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="H16" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="I16" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="J16" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="K16" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="L16" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="M16" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="N16" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="O16" s="30" t="b">
+      <c r="B16" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="C16" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="D16" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="E16" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="F16" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="G16" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="H16" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="I16" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="J16" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="K16" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="L16" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="M16" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="N16" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="O16" s="27" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Working gams file with automatic results output for each solver loop
</commit_message>
<xml_diff>
--- a/ConfigFiles/ConfigTest.xlsx
+++ b/ConfigFiles/ConfigTest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matij\Documents\Github\Heating\Heat-Markets\ConfigFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Github\DARKO\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00B62829-9131-4F4A-804F-A3572C1CEB2D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5287DF7-7A22-43C5-BA1C-D17A0F769591}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -1012,24 +1012,24 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="C68" sqref="C68"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.21875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="16.44140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="68.6640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.44140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="2.44140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="96.33203125" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="30.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="68.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="2.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="96.28515625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="30" t="s">
         <v>118</v>
       </c>
@@ -1041,7 +1041,7 @@
       <c r="G1" s="30"/>
       <c r="H1" s="30"/>
     </row>
-    <row r="2" spans="1:8" ht="3" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="3" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -1051,8 +1051,8 @@
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="29" t="s">
         <v>119</v>
       </c>
@@ -1063,7 +1063,7 @@
       <c r="G4" s="29"/>
       <c r="H4" s="29"/>
     </row>
-    <row r="5" spans="1:8" s="8" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" s="8" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="16"/>
       <c r="C5" s="16"/>
@@ -1073,7 +1073,7 @@
       <c r="G5" s="16"/>
       <c r="H5" s="16"/>
     </row>
-    <row r="6" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>44</v>
       </c>
@@ -1087,7 +1087,7 @@
       <c r="G6" s="28"/>
       <c r="H6" s="28"/>
     </row>
-    <row r="7" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
       <c r="D7" s="12"/>
@@ -1096,20 +1096,20 @@
       <c r="G7" s="12"/>
       <c r="H7" s="12"/>
     </row>
-    <row r="8" spans="1:8" s="8" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" s="8" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="C8" s="14"/>
     </row>
-    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>34</v>
       </c>
@@ -1124,7 +1124,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>31</v>
       </c>
@@ -1138,7 +1138,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>32</v>
       </c>
@@ -1152,7 +1152,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>33</v>
       </c>
@@ -1166,7 +1166,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>65</v>
       </c>
@@ -1177,7 +1177,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>100</v>
       </c>
@@ -1189,17 +1189,17 @@
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="25" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="26" spans="1:8" ht="9" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="28" spans="1:8" ht="3" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="29" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:8" ht="9" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:8" ht="3" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
       <c r="C30" s="14"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>37</v>
       </c>
@@ -1213,7 +1213,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>38</v>
       </c>
@@ -1221,13 +1221,13 @@
         <v>36</v>
       </c>
       <c r="C32" s="18">
-        <v>42371</v>
+        <v>42379</v>
       </c>
       <c r="H32" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>41</v>
       </c>
@@ -1235,13 +1235,13 @@
         <v>42</v>
       </c>
       <c r="C33" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H33" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>43</v>
       </c>
@@ -1252,23 +1252,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="38" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="39" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="42" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="45" spans="1:8" s="8" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:8" s="8" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="7"/>
       <c r="C45" s="14"/>
     </row>
-    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="C46" s="1"/>
     </row>
-    <row r="47" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>39</v>
       </c>
@@ -1282,7 +1282,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>50</v>
       </c>
@@ -1296,25 +1296,25 @@
         <v>52</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="9" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="50" spans="1:8" ht="9.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="51" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="52" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="53" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="54" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="55" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="56" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="57" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="59" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="60" spans="1:8" s="10" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" ht="9" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" spans="1:8" ht="9.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="52" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="54" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="55" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="59" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="60" spans="1:8" s="10" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="9"/>
       <c r="C60" s="15"/>
     </row>
-    <row r="61" spans="1:8" s="8" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" s="8" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="7"/>
       <c r="C61" s="14"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>136</v>
       </c>
@@ -1331,7 +1331,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>137</v>
       </c>
@@ -1348,7 +1348,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>138</v>
       </c>
@@ -1365,7 +1365,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>139</v>
       </c>
@@ -1383,7 +1383,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>128</v>
       </c>
@@ -1400,7 +1400,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>129</v>
       </c>
@@ -1417,7 +1417,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>123</v>
       </c>
@@ -1435,7 +1435,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>131</v>
       </c>
@@ -1453,7 +1453,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>132</v>
       </c>
@@ -1465,7 +1465,7 @@
       </c>
       <c r="D70" s="19"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>133</v>
       </c>
@@ -1479,7 +1479,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>146</v>
       </c>
@@ -1493,7 +1493,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>149</v>
       </c>
@@ -1504,23 +1504,23 @@
         <v>148</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="75" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="76" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="77" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="78" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="79" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="80" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="81" spans="1:6" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="82" spans="1:6" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="83" spans="1:6" ht="4.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="84" spans="1:6" ht="9" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="85" spans="1:6" s="10" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="76" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="77" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="78" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="79" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="80" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="81" spans="1:6" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="82" spans="1:6" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="83" spans="1:6" ht="4.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="84" spans="1:6" ht="9" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="85" spans="1:6" s="10" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="9"/>
       <c r="C85" s="15"/>
     </row>
-    <row r="86" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="87" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="87" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="22" t="s">
         <v>126</v>
       </c>
@@ -1537,7 +1537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="29" t="s">
         <v>45</v>
       </c>
@@ -1554,7 +1554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="29"/>
       <c r="B89" s="6" t="s">
         <v>20</v>
@@ -1569,7 +1569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="29"/>
       <c r="B90" s="6" t="s">
         <v>106</v>
@@ -1584,7 +1584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="29"/>
       <c r="B91" s="6" t="s">
         <v>101</v>
@@ -1599,7 +1599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="29"/>
       <c r="B92" s="6" t="s">
         <v>3</v>
@@ -1614,7 +1614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="29"/>
       <c r="B93" s="6" t="s">
         <v>114</v>
@@ -1629,7 +1629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="29"/>
       <c r="B94" s="6" t="s">
         <v>29</v>
@@ -1644,7 +1644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="29"/>
       <c r="B95" s="6" t="s">
         <v>14</v>
@@ -1659,7 +1659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="29"/>
       <c r="B96" s="6" t="s">
         <v>4</v>
@@ -1674,7 +1674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="29"/>
       <c r="B97" s="6" t="s">
         <v>6</v>
@@ -1689,7 +1689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="29"/>
       <c r="B98" s="6" t="s">
         <v>5</v>
@@ -1704,7 +1704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="29"/>
       <c r="B99" s="6" t="s">
         <v>7</v>
@@ -1719,7 +1719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="29"/>
       <c r="B100" s="6" t="s">
         <v>9</v>
@@ -1734,7 +1734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="29"/>
       <c r="B101" s="6" t="s">
         <v>10</v>
@@ -1749,7 +1749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="29"/>
       <c r="B102" s="6" t="s">
         <v>26</v>
@@ -1764,7 +1764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B103" s="6" t="s">
         <v>11</v>
       </c>
@@ -1778,7 +1778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B104" s="6" t="s">
         <v>12</v>
       </c>
@@ -1792,7 +1792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B105" s="6" t="s">
         <v>18</v>
       </c>
@@ -1806,7 +1806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B106" s="6" t="s">
         <v>8</v>
       </c>
@@ -1823,7 +1823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B107" s="6" t="s">
         <v>111</v>
       </c>
@@ -1840,7 +1840,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="108" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B108" s="6" t="s">
         <v>13</v>
       </c>
@@ -1854,16 +1854,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109" s="9"/>
       <c r="C109" s="15"/>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
         <v>1</v>
       </c>
@@ -1874,7 +1874,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>59</v>
       </c>
@@ -1888,7 +1888,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>60</v>
       </c>
@@ -1902,7 +1902,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>62</v>
       </c>
@@ -1913,28 +1913,28 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="117" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="118" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="119" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="120" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="121" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="122" spans="1:8" ht="3.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="123" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="124" spans="1:8" ht="1.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="125" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="126" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="127" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="128" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="117" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="118" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="119" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="120" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="121" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="122" spans="1:8" ht="3.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="123" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="124" spans="1:8" ht="1.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="125" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="126" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="127" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="128" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A128" s="9"/>
       <c r="C128" s="15"/>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B132" s="24" t="s">
         <v>70</v>
       </c>
@@ -1942,7 +1942,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B133" s="24" t="s">
         <v>71</v>
       </c>
@@ -1950,7 +1950,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B134" s="24" t="s">
         <v>72</v>
       </c>
@@ -1958,7 +1958,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B135" s="24" t="s">
         <v>73</v>
       </c>
@@ -1966,7 +1966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B136" s="24" t="s">
         <v>74</v>
       </c>
@@ -1974,7 +1974,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B137" s="24" t="s">
         <v>75</v>
       </c>
@@ -1982,7 +1982,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B138" s="24" t="s">
         <v>76</v>
       </c>
@@ -1990,7 +1990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B139" s="24" t="s">
         <v>77</v>
       </c>
@@ -1998,7 +1998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B140" s="24" t="s">
         <v>78</v>
       </c>
@@ -2006,7 +2006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B141" s="24" t="s">
         <v>79</v>
       </c>
@@ -2014,7 +2014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B142" s="24" t="s">
         <v>80</v>
       </c>
@@ -2022,7 +2022,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B143" s="24" t="s">
         <v>81</v>
       </c>
@@ -2030,7 +2030,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B144" s="24" t="s">
         <v>82</v>
       </c>
@@ -2038,7 +2038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="145" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B145" s="24" t="s">
         <v>83</v>
       </c>
@@ -2046,7 +2046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="146" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B146" s="24" t="s">
         <v>84</v>
       </c>
@@ -2054,7 +2054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="165" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F165" s="2"/>
     </row>
   </sheetData>
@@ -2150,14 +2150,14 @@
       <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" customWidth="1"/>
-    <col min="2" max="2" width="32.5546875" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="32.5703125" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>2</v>
       </c>
@@ -2168,7 +2168,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="b">
         <v>1</v>
       </c>
@@ -2179,7 +2179,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="b">
         <v>0</v>
       </c>
@@ -2199,12 +2199,12 @@
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="17"/>
+    <col min="1" max="1" width="9.140625" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="26"/>
       <c r="B1" s="26" t="s">
         <v>85</v>
@@ -2249,7 +2249,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
         <v>70</v>
       </c>
@@ -2296,7 +2296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
         <v>71</v>
       </c>
@@ -2343,7 +2343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
         <v>72</v>
       </c>
@@ -2390,7 +2390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
         <v>73</v>
       </c>
@@ -2437,7 +2437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
         <v>74</v>
       </c>
@@ -2484,7 +2484,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
         <v>75</v>
       </c>
@@ -2531,7 +2531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
         <v>76</v>
       </c>
@@ -2578,7 +2578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
         <v>77</v>
       </c>
@@ -2625,7 +2625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="26" t="s">
         <v>78</v>
       </c>
@@ -2672,7 +2672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="26" t="s">
         <v>79</v>
       </c>
@@ -2719,7 +2719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="26" t="s">
         <v>80</v>
       </c>
@@ -2766,7 +2766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="26" t="s">
         <v>81</v>
       </c>
@@ -2813,7 +2813,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="26" t="s">
         <v>82</v>
       </c>
@@ -2860,7 +2860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="26" t="s">
         <v>83</v>
       </c>
@@ -2907,7 +2907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="26" t="s">
         <v>84</v>
       </c>

</xml_diff>

<commit_message>
Ramping limits included in the model and updated input parameters
</commit_message>
<xml_diff>
--- a/ConfigFiles/ConfigTest.xlsx
+++ b/ConfigFiles/ConfigTest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Github\DARKO\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5287DF7-7A22-43C5-BA1C-D17A0F769591}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AE9D39A-2D63-4BB2-B345-73E8FF401FD4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="161">
   <si>
     <t>Default value</t>
   </si>
@@ -489,6 +491,30 @@
   </si>
   <si>
     <t>Database/Price/##/PriceSimpleOrder.csv</t>
+  </si>
+  <si>
+    <t>Line - Daily Ramp Up</t>
+  </si>
+  <si>
+    <t>Line - Daily Ramp Down</t>
+  </si>
+  <si>
+    <t>Line - Hourly Ramp Up</t>
+  </si>
+  <si>
+    <t>Line - Hourly Ramp Down</t>
+  </si>
+  <si>
+    <t>Node - Daily Ramp Up</t>
+  </si>
+  <si>
+    <t>Node - Daily Ramp Down</t>
+  </si>
+  <si>
+    <t>Node - Hourly Ramp Up</t>
+  </si>
+  <si>
+    <t>Node - Hourly Ramp Down</t>
   </si>
 </sst>
 </file>
@@ -1012,8 +1038,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H165"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="F81" sqref="F81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,20 +1122,20 @@
       <c r="G7" s="12"/>
       <c r="H7" s="12"/>
     </row>
-    <row r="8" spans="1:8" s="8" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" s="8" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="C8" s="14"/>
     </row>
-    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>34</v>
       </c>
@@ -1124,7 +1150,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>31</v>
       </c>
@@ -1138,7 +1164,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>32</v>
       </c>
@@ -1152,7 +1178,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>33</v>
       </c>
@@ -1166,7 +1192,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>65</v>
       </c>
@@ -1177,7 +1203,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>100</v>
       </c>
@@ -1189,17 +1215,17 @@
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:8" ht="9" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:8" ht="3" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:8" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
       <c r="C30" s="14"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>37</v>
       </c>
@@ -1213,7 +1239,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>38</v>
       </c>
@@ -1227,7 +1253,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>41</v>
       </c>
@@ -1241,7 +1267,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>43</v>
       </c>
@@ -1252,20 +1278,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="38" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="1:8" s="8" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:8" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="7"/>
       <c r="C45" s="14"/>
     </row>
-    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C46" s="1"/>
     </row>
     <row r="47" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1296,25 +1323,26 @@
         <v>52</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="9" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="50" spans="1:8" ht="9.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="52" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="53" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="54" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="55" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="56" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="57" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="59" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="60" spans="1:8" s="10" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" spans="1:8" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="9"/>
       <c r="C60" s="15"/>
     </row>
-    <row r="61" spans="1:8" s="8" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="7"/>
       <c r="C61" s="14"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>136</v>
       </c>
@@ -1331,7 +1359,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>137</v>
       </c>
@@ -1348,7 +1376,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>138</v>
       </c>
@@ -1365,7 +1393,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>139</v>
       </c>
@@ -1383,7 +1411,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>128</v>
       </c>
@@ -1400,7 +1428,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>129</v>
       </c>
@@ -1417,7 +1445,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>123</v>
       </c>
@@ -1435,7 +1463,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>131</v>
       </c>
@@ -1453,7 +1481,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>132</v>
       </c>
@@ -1465,7 +1493,7 @@
       </c>
       <c r="D70" s="19"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>133</v>
       </c>
@@ -1479,7 +1507,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>146</v>
       </c>
@@ -1493,7 +1521,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>149</v>
       </c>
@@ -1504,23 +1532,103 @@
         <v>148</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="75" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="76" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="77" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="78" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="79" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="80" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="81" spans="1:6" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="82" spans="1:6" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="83" spans="1:6" ht="4.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="84" spans="1:6" ht="9" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="85" spans="1:6" s="10" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F74" s="5">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F75" s="5">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F76" s="5">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F77" s="5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F78" s="5">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F79" s="5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F80" s="5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F81" s="5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="83" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="84" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="85" spans="1:6" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="9"/>
       <c r="C85" s="15"/>
     </row>
-    <row r="86" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="87" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="87" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="22" t="s">
         <v>126</v>
       </c>
@@ -1537,7 +1645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="29" t="s">
         <v>45</v>
       </c>
@@ -1554,7 +1662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="29"/>
       <c r="B89" s="6" t="s">
         <v>20</v>
@@ -1569,7 +1677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="29"/>
       <c r="B90" s="6" t="s">
         <v>106</v>
@@ -1584,7 +1692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="29"/>
       <c r="B91" s="6" t="s">
         <v>101</v>
@@ -1599,7 +1707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="29"/>
       <c r="B92" s="6" t="s">
         <v>3</v>
@@ -1614,7 +1722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="29"/>
       <c r="B93" s="6" t="s">
         <v>114</v>
@@ -1629,7 +1737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="29"/>
       <c r="B94" s="6" t="s">
         <v>29</v>
@@ -1644,7 +1752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="29"/>
       <c r="B95" s="6" t="s">
         <v>14</v>
@@ -1659,7 +1767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="29"/>
       <c r="B96" s="6" t="s">
         <v>4</v>
@@ -1674,7 +1782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="29"/>
       <c r="B97" s="6" t="s">
         <v>6</v>
@@ -1689,7 +1797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="29"/>
       <c r="B98" s="6" t="s">
         <v>5</v>
@@ -1704,7 +1812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="29"/>
       <c r="B99" s="6" t="s">
         <v>7</v>
@@ -1719,7 +1827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="29"/>
       <c r="B100" s="6" t="s">
         <v>9</v>
@@ -1734,7 +1842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="29"/>
       <c r="B101" s="6" t="s">
         <v>10</v>
@@ -1749,7 +1857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="29"/>
       <c r="B102" s="6" t="s">
         <v>26</v>
@@ -1764,7 +1872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B103" s="6" t="s">
         <v>11</v>
       </c>
@@ -1778,7 +1886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B104" s="6" t="s">
         <v>12</v>
       </c>
@@ -1792,7 +1900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B105" s="6" t="s">
         <v>18</v>
       </c>
@@ -1806,7 +1914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B106" s="6" t="s">
         <v>8</v>
       </c>
@@ -1823,7 +1931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B107" s="6" t="s">
         <v>111</v>
       </c>
@@ -1840,7 +1948,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="108" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B108" s="6" t="s">
         <v>13</v>
       </c>
@@ -1854,16 +1962,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="9"/>
       <c r="C109" s="15"/>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="111" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
         <v>1</v>
       </c>
@@ -1874,7 +1983,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>59</v>
       </c>
@@ -1888,7 +1997,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>60</v>
       </c>
@@ -1902,7 +2011,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>62</v>
       </c>
@@ -1913,28 +2022,30 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="117" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="118" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="119" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="120" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="121" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="122" spans="1:8" ht="3.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="123" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="124" spans="1:8" ht="1.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="125" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="126" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="127" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="128" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="117" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="118" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="119" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="120" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="121" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="122" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="123" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="124" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="125" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="126" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="127" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="128" spans="1:8" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="9"/>
       <c r="C128" s="15"/>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="130" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="132" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B132" s="24" t="s">
         <v>70</v>
       </c>
@@ -1942,7 +2053,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B133" s="24" t="s">
         <v>71</v>
       </c>
@@ -1950,7 +2061,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B134" s="24" t="s">
         <v>72</v>
       </c>
@@ -1958,7 +2069,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B135" s="24" t="s">
         <v>73</v>
       </c>
@@ -1966,7 +2077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B136" s="24" t="s">
         <v>74</v>
       </c>
@@ -1974,7 +2085,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B137" s="24" t="s">
         <v>75</v>
       </c>
@@ -1982,7 +2093,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B138" s="24" t="s">
         <v>76</v>
       </c>
@@ -1990,7 +2101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B139" s="24" t="s">
         <v>77</v>
       </c>
@@ -1998,7 +2109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B140" s="24" t="s">
         <v>78</v>
       </c>
@@ -2006,7 +2117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B141" s="24" t="s">
         <v>79</v>
       </c>
@@ -2014,7 +2125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B142" s="24" t="s">
         <v>80</v>
       </c>
@@ -2022,7 +2133,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B143" s="24" t="s">
         <v>81</v>
       </c>
@@ -2030,7 +2141,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B144" s="24" t="s">
         <v>82</v>
       </c>
@@ -2038,7 +2149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B145" s="24" t="s">
         <v>83</v>
       </c>
@@ -2046,7 +2157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B146" s="24" t="s">
         <v>84</v>
       </c>
@@ -2054,6 +2165,8 @@
         <v>0</v>
       </c>
     </row>
+    <row r="147" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="148" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="165" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F165" s="2"/>
     </row>
@@ -2082,7 +2195,7 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Multiplicative Factor" prompt="This modifier multiplies the PV generation curves of all the zones by the provided factor" sqref="C114" xr:uid="{00000000-0002-0000-0000-000007000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Multiplicative Factor" prompt="This modifier multiplies the storage capacity in all the zones by the provided factor" sqref="C115" xr:uid="{00000000-0002-0000-0000-000008000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to the gams folder" prompt="Example:_x000a_C:\GAMS\win64\24.3_x000a__x000a_If unspecified or non-existing, Dispa-SET will try to determine the path automatically. " sqref="C22" xr:uid="{00000000-0002-0000-0000-000009000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default value (% of max load)" prompt="In case no data file is provided. This single value is used for all the sets._x000a_It is defined in % of the maximum load throughout the simulation period." sqref="F68:F69 F65" xr:uid="{56B7C1C7-C83A-40F5-A03D-AFAA1755A969}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default value (% of max load)" prompt="In case no data file is provided. This single value is used for all the sets._x000a_It is defined in % of the maximum load throughout the simulation period." sqref="F68:F69 F65 F74:F81" xr:uid="{56B7C1C7-C83A-40F5-A03D-AFAA1755A969}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to the cplex executable" prompt="This is only useful if the Pyomo engine is selected and if cplex is not in the PATH (i.e. accessible from the prompt). This parameters can be left unspecified in most cases._x000a__x000a_Example:_x000a_C:\\Users\\ese-veda06\\Downloads\\solvers\\cplex.exe" sqref="C23" xr:uid="{00000000-0002-0000-0000-00000C000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path the outage data" prompt="Select the path the outage csv file from the database._x000a__x000a_The path should be relative to this excel file. Use &quot;..&quot; to go up one folder. Folder separator can be either &quot;/&quot; or &quot;\&quot;" sqref="C63" xr:uid="{00000000-0002-0000-0000-00000E000000}"/>
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Look Ahead Period" prompt="This is the overlap period between consecutive optimization of the rolling horizon._x000a__x000a_If HorizonLength is 3 and  LookAhead is 1, optimization length is 4 days, discarding 1 day each time" sqref="C34" xr:uid="{00000000-0002-0000-0000-00000F000000}">

</xml_diff>

<commit_message>
Results now saved as excel files
</commit_message>
<xml_diff>
--- a/ConfigFiles/ConfigTest.xlsx
+++ b/ConfigFiles/ConfigTest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Github\DARKO\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AE9D39A-2D63-4BB2-B345-73E8FF401FD4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C63EDB37-E0E8-442F-ACD9-1DEE10C73A6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1038,8 +1038,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="F81" sqref="F81"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1158,7 +1158,7 @@
         <v>2</v>
       </c>
       <c r="C19" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>53</v>

</xml_diff>

<commit_message>
Unit Ramping limits, new fuel + technology combinations, code cleanup
</commit_message>
<xml_diff>
--- a/ConfigFiles/ConfigTest.xlsx
+++ b/ConfigFiles/ConfigTest.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Github\DARKO\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D2A6DA1-A113-42C0-8E97-2AA55623CC66}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{654995FB-5839-4720-BEBF-077AC28682D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -463,82 +463,82 @@
     <t>Database/Availability/##/DemandOrder.csv</t>
   </si>
   <si>
+    <t>Database/Availability/##/SimpleOrder.csv</t>
+  </si>
+  <si>
+    <t>..Database/Availability/##/DemandOrder.csv</t>
+  </si>
+  <si>
+    <t>Interconnections</t>
+  </si>
+  <si>
+    <t>EUR/MWh</t>
+  </si>
+  <si>
+    <t>Database/Interconnections/NTC/NTC.csv</t>
+  </si>
+  <si>
+    <t>NTC</t>
+  </si>
+  <si>
+    <t>Database/Interconnections/CBF/CBF.csv</t>
+  </si>
+  <si>
+    <t>Database/Price/##/PriceDemandOrder.csv</t>
+  </si>
+  <si>
+    <t>Database/Price/##/PriceSimpleOrder.csv</t>
+  </si>
+  <si>
+    <t>Line - Daily Ramp Up</t>
+  </si>
+  <si>
+    <t>Line - Daily Ramp Down</t>
+  </si>
+  <si>
+    <t>Line - Hourly Ramp Up</t>
+  </si>
+  <si>
+    <t>Line - Hourly Ramp Down</t>
+  </si>
+  <si>
+    <t>Node - Daily Ramp Up</t>
+  </si>
+  <si>
+    <t>Node - Daily Ramp Down</t>
+  </si>
+  <si>
+    <t>Node - Hourly Ramp Up</t>
+  </si>
+  <si>
+    <t>Node - Hourly Ramp Down</t>
+  </si>
+  <si>
+    <t>AD</t>
+  </si>
+  <si>
+    <t>AL</t>
+  </si>
+  <si>
+    <t>HOBO</t>
+  </si>
+  <si>
+    <t>HEPU</t>
+  </si>
+  <si>
+    <t>ELHE</t>
+  </si>
+  <si>
+    <t>SOTH</t>
+  </si>
+  <si>
+    <t>GETH</t>
+  </si>
+  <si>
+    <t>WSHE</t>
+  </si>
+  <si>
     <t>Database/Availability/##/BlockOrder.csv</t>
-  </si>
-  <si>
-    <t>Database/Availability/##/SimpleOrder.csv</t>
-  </si>
-  <si>
-    <t>..Database/Availability/##/DemandOrder.csv</t>
-  </si>
-  <si>
-    <t>Interconnections</t>
-  </si>
-  <si>
-    <t>EUR/MWh</t>
-  </si>
-  <si>
-    <t>Database/Interconnections/NTC/NTC.csv</t>
-  </si>
-  <si>
-    <t>NTC</t>
-  </si>
-  <si>
-    <t>Database/Interconnections/CBF/CBF.csv</t>
-  </si>
-  <si>
-    <t>Database/Price/##/PriceDemandOrder.csv</t>
-  </si>
-  <si>
-    <t>Database/Price/##/PriceSimpleOrder.csv</t>
-  </si>
-  <si>
-    <t>Line - Daily Ramp Up</t>
-  </si>
-  <si>
-    <t>Line - Daily Ramp Down</t>
-  </si>
-  <si>
-    <t>Line - Hourly Ramp Up</t>
-  </si>
-  <si>
-    <t>Line - Hourly Ramp Down</t>
-  </si>
-  <si>
-    <t>Node - Daily Ramp Up</t>
-  </si>
-  <si>
-    <t>Node - Daily Ramp Down</t>
-  </si>
-  <si>
-    <t>Node - Hourly Ramp Up</t>
-  </si>
-  <si>
-    <t>Node - Hourly Ramp Down</t>
-  </si>
-  <si>
-    <t>AD</t>
-  </si>
-  <si>
-    <t>AL</t>
-  </si>
-  <si>
-    <t>HOBO</t>
-  </si>
-  <si>
-    <t>HEPU</t>
-  </si>
-  <si>
-    <t>ELHE</t>
-  </si>
-  <si>
-    <t>SOTH</t>
-  </si>
-  <si>
-    <t>GETH</t>
-  </si>
-  <si>
-    <t>WSHE</t>
   </si>
 </sst>
 </file>
@@ -713,6 +713,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -720,12 +726,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1068,8 +1068,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A105" workbookViewId="0">
-      <selection activeCell="F147" sqref="F147"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1086,16 +1086,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="32" t="s">
         <v>118</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
     </row>
     <row r="2" spans="1:8" ht="3" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
@@ -1109,15 +1109,15 @@
     </row>
     <row r="3" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="31" t="s">
         <v>119</v>
       </c>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="29"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
     </row>
     <row r="5" spans="1:8" s="8" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
@@ -1133,15 +1133,15 @@
       <c r="A6" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="30" t="s">
         <v>120</v>
       </c>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="28"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
     </row>
     <row r="7" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="12"/>
@@ -1397,7 +1397,7 @@
         <v>35</v>
       </c>
       <c r="C63" s="21" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D63" s="19" t="s">
         <v>69</v>
@@ -1413,8 +1413,8 @@
       <c r="B64" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C64" s="20" t="s">
-        <v>143</v>
+      <c r="C64" s="21" t="s">
+        <v>168</v>
       </c>
       <c r="D64" s="19" t="s">
         <v>69</v>
@@ -1449,13 +1449,13 @@
         <v>35</v>
       </c>
       <c r="C66" s="20" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D66" s="19" t="s">
         <v>69</v>
       </c>
       <c r="H66" s="11" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="67" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1466,7 +1466,7 @@
         <v>35</v>
       </c>
       <c r="C67" s="20" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D67" s="19" t="s">
         <v>69</v>
@@ -1490,7 +1490,7 @@
         <v>30</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="69" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1508,7 +1508,7 @@
         <v>50</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="70" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1539,13 +1539,13 @@
     </row>
     <row r="72" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C72" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D72" s="19" t="s">
         <v>69</v>
@@ -1553,18 +1553,18 @@
     </row>
     <row r="73" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C73" s="20" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="74" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E74" s="1" t="s">
         <v>0</v>
@@ -1575,7 +1575,7 @@
     </row>
     <row r="75" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>0</v>
@@ -1586,7 +1586,7 @@
     </row>
     <row r="76" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>0</v>
@@ -1597,7 +1597,7 @@
     </row>
     <row r="77" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>0</v>
@@ -1608,7 +1608,7 @@
     </row>
     <row r="78" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E78" s="1" t="s">
         <v>0</v>
@@ -1619,7 +1619,7 @@
     </row>
     <row r="79" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>0</v>
@@ -1630,7 +1630,7 @@
     </row>
     <row r="80" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E80" s="1" t="s">
         <v>0</v>
@@ -1641,7 +1641,7 @@
     </row>
     <row r="81" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E81" s="1" t="s">
         <v>0</v>
@@ -1663,7 +1663,7 @@
         <v>126</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C87" s="4" t="b">
         <v>0</v>
@@ -1676,11 +1676,11 @@
       </c>
     </row>
     <row r="88" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="29" t="s">
+      <c r="A88" s="31" t="s">
         <v>45</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C88" s="4" t="b">
         <v>0</v>
@@ -1693,7 +1693,7 @@
       </c>
     </row>
     <row r="89" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="29"/>
+      <c r="A89" s="31"/>
       <c r="B89" s="6" t="s">
         <v>20</v>
       </c>
@@ -1708,7 +1708,7 @@
       </c>
     </row>
     <row r="90" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="29"/>
+      <c r="A90" s="31"/>
       <c r="B90" s="6" t="s">
         <v>106</v>
       </c>
@@ -1723,7 +1723,7 @@
       </c>
     </row>
     <row r="91" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="29"/>
+      <c r="A91" s="31"/>
       <c r="B91" s="6" t="s">
         <v>101</v>
       </c>
@@ -1738,7 +1738,7 @@
       </c>
     </row>
     <row r="92" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="29"/>
+      <c r="A92" s="31"/>
       <c r="B92" s="6" t="s">
         <v>3</v>
       </c>
@@ -1753,7 +1753,7 @@
       </c>
     </row>
     <row r="93" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="29"/>
+      <c r="A93" s="31"/>
       <c r="B93" s="6" t="s">
         <v>114</v>
       </c>
@@ -1768,7 +1768,7 @@
       </c>
     </row>
     <row r="94" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="29"/>
+      <c r="A94" s="31"/>
       <c r="B94" s="6" t="s">
         <v>29</v>
       </c>
@@ -1783,7 +1783,7 @@
       </c>
     </row>
     <row r="95" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="29"/>
+      <c r="A95" s="31"/>
       <c r="B95" s="6" t="s">
         <v>14</v>
       </c>
@@ -1798,7 +1798,7 @@
       </c>
     </row>
     <row r="96" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="29"/>
+      <c r="A96" s="31"/>
       <c r="B96" s="6" t="s">
         <v>4</v>
       </c>
@@ -1813,7 +1813,7 @@
       </c>
     </row>
     <row r="97" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="29"/>
+      <c r="A97" s="31"/>
       <c r="B97" s="6" t="s">
         <v>6</v>
       </c>
@@ -1828,7 +1828,7 @@
       </c>
     </row>
     <row r="98" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="29"/>
+      <c r="A98" s="31"/>
       <c r="B98" s="6" t="s">
         <v>5</v>
       </c>
@@ -1843,7 +1843,7 @@
       </c>
     </row>
     <row r="99" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="29"/>
+      <c r="A99" s="31"/>
       <c r="B99" s="6" t="s">
         <v>7</v>
       </c>
@@ -1858,7 +1858,7 @@
       </c>
     </row>
     <row r="100" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="29"/>
+      <c r="A100" s="31"/>
       <c r="B100" s="6" t="s">
         <v>9</v>
       </c>
@@ -1873,7 +1873,7 @@
       </c>
     </row>
     <row r="101" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="29"/>
+      <c r="A101" s="31"/>
       <c r="B101" s="6" t="s">
         <v>10</v>
       </c>
@@ -1888,7 +1888,7 @@
       </c>
     </row>
     <row r="102" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="29"/>
+      <c r="A102" s="31"/>
       <c r="B102" s="6" t="s">
         <v>26</v>
       </c>
@@ -2194,10 +2194,10 @@
       </c>
     </row>
     <row r="146" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B146" s="32" t="s">
+      <c r="B146" s="29" t="s">
         <v>83</v>
       </c>
-      <c r="C146" s="31" t="b">
+      <c r="C146" s="28" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2210,50 +2210,50 @@
       </c>
     </row>
     <row r="148" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B148" s="32" t="s">
+      <c r="B148" s="29" t="s">
+        <v>162</v>
+      </c>
+      <c r="C148" s="28" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B149" s="29" t="s">
         <v>163</v>
       </c>
-      <c r="C148" s="31" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="149" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B149" s="32" t="s">
+      <c r="C149" s="28" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B150" s="29" t="s">
         <v>164</v>
       </c>
-      <c r="C149" s="31" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="150" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B150" s="32" t="s">
+      <c r="C150" s="28" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B151" s="29" t="s">
         <v>165</v>
       </c>
-      <c r="C150" s="31" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="151" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B151" s="32" t="s">
+      <c r="C151" s="28" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B152" s="29" t="s">
         <v>166</v>
       </c>
-      <c r="C151" s="31" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="152" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B152" s="32" t="s">
+      <c r="C152" s="28" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B153" s="29" t="s">
         <v>167</v>
       </c>
-      <c r="C152" s="31" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="153" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B153" s="32" t="s">
-        <v>168</v>
-      </c>
-      <c r="C153" s="31" t="b">
+      <c r="C153" s="28" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2286,7 +2286,7 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Multiplicative Factor" prompt="This modifier multiplies the storage capacity in all the zones by the provided factor" sqref="C116" xr:uid="{00000000-0002-0000-0000-000008000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to the gams folder" prompt="Example:_x000a_C:\GAMS\win64\24.3_x000a__x000a_If unspecified or non-existing, DARKO will try to determine the path automatically. " sqref="C22" xr:uid="{00000000-0002-0000-0000-000009000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to the cplex executable" prompt="This is only useful if the Pyomo engine is selected and if cplex is not in the PATH (i.e. accessible from the prompt). This parameters can be left unspecified in most cases._x000a__x000a_Example:_x000a_C:\\Users\\ese-veda06\\Downloads\\solvers\\cplex.exe" sqref="C23" xr:uid="{00000000-0002-0000-0000-00000C000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path the Simple Order data" prompt="Select the path the Simple Order csv file from the database._x000a__x000a_The path should be relative to this excel file. Use &quot;..&quot; to go up one folder. Folder separator can be either &quot;/&quot; or &quot;\&quot;" sqref="C63" xr:uid="{00000000-0002-0000-0000-00000E000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path the Simple Order data" prompt="Select the path the Simple Order csv file from the database._x000a__x000a_The path should be relative to this excel file. Use &quot;..&quot; to go up one folder. Folder separator can be either &quot;/&quot; or &quot;\&quot;" sqref="C63:C64" xr:uid="{00000000-0002-0000-0000-00000E000000}"/>
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Look Ahead Period" prompt="This is the overlap period between consecutive optimization of the rolling horizon._x000a__x000a_If HorizonLength is 3 and  LookAhead is 1, optimization length is 4 days, discarding 1 day each time" sqref="C34" xr:uid="{00000000-0002-0000-0000-00000F000000}">
       <formula1>0</formula1>
       <formula2>365</formula2>

</xml_diff>

<commit_message>
Preprocessing setup for Storage
</commit_message>
<xml_diff>
--- a/ConfigFiles/ConfigTest.xlsx
+++ b/ConfigFiles/ConfigTest.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Github\DARKO\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{654995FB-5839-4720-BEBF-077AC28682D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF901BA5-8232-4209-B5E8-FAC963971407}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10725" yWindow="2130" windowWidth="11895" windowHeight="11055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
     <sheet name="Lists" sheetId="2" r:id="rId2"/>
     <sheet name="ReserveParticipation" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" calcOnSave="0"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="172">
   <si>
     <t>Default value</t>
   </si>
@@ -539,6 +540,15 @@
   </si>
   <si>
     <t>Database/Availability/##/BlockOrder.csv</t>
+  </si>
+  <si>
+    <t>Storage Inflows</t>
+  </si>
+  <si>
+    <t>Storage Profiles</t>
+  </si>
+  <si>
+    <t>Database/Storage/Profiles/##/Profiles.csv</t>
   </si>
 </sst>
 </file>
@@ -1068,8 +1078,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C65" sqref="C65"/>
+    <sheetView tabSelected="1" topLeftCell="B72" workbookViewId="0">
+      <selection activeCell="C82" sqref="C82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1650,8 +1660,26 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="82" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="83" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="82" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C82" s="20"/>
+    </row>
+    <row r="83" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C83" s="20" t="s">
+        <v>171</v>
+      </c>
+    </row>
     <row r="84" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="85" spans="1:6" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="9"/>

</xml_diff>

<commit_message>
Storage level fix and new outputs
</commit_message>
<xml_diff>
--- a/ConfigFiles/ConfigTest.xlsx
+++ b/ConfigFiles/ConfigTest.xlsx
@@ -8,17 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Github\DARKO\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF901BA5-8232-4209-B5E8-FAC963971407}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64E1C692-88B8-4B7C-9BDB-CCACA446F906}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10725" yWindow="2130" windowWidth="11895" windowHeight="11055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
     <sheet name="Lists" sheetId="2" r:id="rId2"/>
     <sheet name="ReserveParticipation" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029" calcOnSave="0"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="173">
   <si>
     <t>Default value</t>
   </si>
@@ -549,6 +548,9 @@
   </si>
   <si>
     <t>Database/Storage/Profiles/##/Profiles.csv</t>
+  </si>
+  <si>
+    <t>Database/Storage/InFlows/##/InFlows.csv</t>
   </si>
 </sst>
 </file>
@@ -1667,7 +1669,9 @@
       <c r="B82" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C82" s="20"/>
+      <c r="C82" s="20" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="83" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">

</xml_diff>

<commit_message>
Database changes, minor gams fix and basic plots
</commit_message>
<xml_diff>
--- a/ConfigFiles/ConfigTest.xlsx
+++ b/ConfigFiles/ConfigTest.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23001"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Github\DARKO\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64E1C692-88B8-4B7C-9BDB-CCACA446F906}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4DC63CD-6C5E-4005-8B86-9E4359252E7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1080,8 +1080,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B72" workbookViewId="0">
-      <selection activeCell="C82" sqref="C82"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C87" sqref="C87:C109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
New plots in postprocessing
</commit_message>
<xml_diff>
--- a/ConfigFiles/ConfigTest.xlsx
+++ b/ConfigFiles/ConfigTest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Github\DARKO\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4DC63CD-6C5E-4005-8B86-9E4359252E7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF7458FC-C252-4AA0-84BE-0FD00444597D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1081,7 +1081,7 @@
   <dimension ref="A1:H166"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C87" sqref="C87:C109"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1289,7 +1289,7 @@
         <v>36</v>
       </c>
       <c r="C32" s="18">
-        <v>42379</v>
+        <v>42400</v>
       </c>
       <c r="H32" s="1" t="s">
         <v>57</v>
@@ -1303,7 +1303,7 @@
         <v>42</v>
       </c>
       <c r="C33" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H33" s="1" t="s">
         <v>68</v>

</xml_diff>

<commit_message>
Updates and minor bug fixes
</commit_message>
<xml_diff>
--- a/ConfigFiles/ConfigTest.xlsx
+++ b/ConfigFiles/ConfigTest.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Github\DARKO\ConfigFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Github\DARKO\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F336040C-ED03-41B0-AA02-B4E3B20C3CC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEC47018-159F-421D-972D-520B1CE43234}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -436,12 +436,6 @@
     <t>Players - Supply Side</t>
   </si>
   <si>
-    <t>Database/Players/DemandSide/##/DemandSide.csv</t>
-  </si>
-  <si>
-    <t>Database/Players/SupplySide/##/SupplySide.csv</t>
-  </si>
-  <si>
     <t xml:space="preserve">Availability - Demand Order </t>
   </si>
   <si>
@@ -460,12 +454,6 @@
     <t>Z2</t>
   </si>
   <si>
-    <t>Database/Availability/##/DemandOrder.csv</t>
-  </si>
-  <si>
-    <t>Database/Availability/##/SimpleOrder.csv</t>
-  </si>
-  <si>
     <t>..Database/Availability/##/DemandOrder.csv</t>
   </si>
   <si>
@@ -475,21 +463,9 @@
     <t>EUR/MWh</t>
   </si>
   <si>
-    <t>Database/Interconnections/NTC/NTC.csv</t>
-  </si>
-  <si>
     <t>NTC</t>
   </si>
   <si>
-    <t>Database/Interconnections/CBF/CBF.csv</t>
-  </si>
-  <si>
-    <t>Database/Price/##/PriceDemandOrder.csv</t>
-  </si>
-  <si>
-    <t>Database/Price/##/PriceSimpleOrder.csv</t>
-  </si>
-  <si>
     <t>Line - Daily Ramp Up</t>
   </si>
   <si>
@@ -538,19 +514,43 @@
     <t>WSHE</t>
   </si>
   <si>
-    <t>Database/Availability/##/BlockOrder.csv</t>
-  </si>
-  <si>
     <t>Storage Inflows</t>
   </si>
   <si>
     <t>Storage Profiles</t>
   </si>
   <si>
-    <t>Database/Storage/Profiles/##/Profiles.csv</t>
-  </si>
-  <si>
-    <t>Database/Storage/InFlows/##/InFlows.csv</t>
+    <t>tests/dummy_data/Availability/##/DemandOrder.csv</t>
+  </si>
+  <si>
+    <t>tests/dummy_data/Availability/##/SimpleOrder.csv</t>
+  </si>
+  <si>
+    <t>tests/dummy_data/Availability/##/BlockOrder.csv</t>
+  </si>
+  <si>
+    <t>tests/dummy_data/Price/##/PriceDemandOrder.csv</t>
+  </si>
+  <si>
+    <t>tests/dummy_data/Price/##/PriceSimpleOrder.csv</t>
+  </si>
+  <si>
+    <t>tests/dummy_data/Players/DemandSide/##/DemandSide.csv</t>
+  </si>
+  <si>
+    <t>tests/dummy_data/Players/SupplySide/##/SupplySide.csv</t>
+  </si>
+  <si>
+    <t>tests/dummy_data/Interconnections/CBF/CBF.csv</t>
+  </si>
+  <si>
+    <t>tests/dummy_data/Interconnections/NTC/NTC.csv</t>
+  </si>
+  <si>
+    <t>tests/dummy_data/Storage/InFlows/##/InFlows.csv</t>
+  </si>
+  <si>
+    <t>tests/dummy_data/Storage/Profiles/##/Profiles.csv</t>
   </si>
 </sst>
 </file>
@@ -1080,8 +1080,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H166"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="C84" sqref="C84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1386,13 +1386,13 @@
     </row>
     <row r="62" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C62" s="20" t="s">
-        <v>142</v>
+        <v>162</v>
       </c>
       <c r="D62" s="19" t="s">
         <v>69</v>
@@ -1403,13 +1403,13 @@
     </row>
     <row r="63" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C63" s="21" t="s">
-        <v>143</v>
+        <v>163</v>
       </c>
       <c r="D63" s="19" t="s">
         <v>69</v>
@@ -1420,24 +1420,24 @@
     </row>
     <row r="64" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C64" s="21" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D64" s="19" t="s">
         <v>69</v>
       </c>
       <c r="H64" s="11" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="65" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C65" s="1"/>
       <c r="D65" s="19" t="s">
@@ -1461,13 +1461,13 @@
         <v>35</v>
       </c>
       <c r="C66" s="20" t="s">
-        <v>150</v>
+        <v>165</v>
       </c>
       <c r="D66" s="19" t="s">
         <v>69</v>
       </c>
       <c r="H66" s="11" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="67" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1478,7 +1478,7 @@
         <v>35</v>
       </c>
       <c r="C67" s="20" t="s">
-        <v>151</v>
+        <v>166</v>
       </c>
       <c r="D67" s="19" t="s">
         <v>69</v>
@@ -1502,7 +1502,7 @@
         <v>30</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="69" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1520,7 +1520,7 @@
         <v>50</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="70" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1531,7 +1531,7 @@
         <v>35</v>
       </c>
       <c r="C70" s="20" t="s">
-        <v>134</v>
+        <v>167</v>
       </c>
       <c r="D70" s="19"/>
     </row>
@@ -1543,7 +1543,7 @@
         <v>35</v>
       </c>
       <c r="C71" s="20" t="s">
-        <v>135</v>
+        <v>168</v>
       </c>
       <c r="D71" s="19" t="s">
         <v>69</v>
@@ -1551,13 +1551,13 @@
     </row>
     <row r="72" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C72" s="20" t="s">
-        <v>149</v>
+        <v>169</v>
       </c>
       <c r="D72" s="19" t="s">
         <v>69</v>
@@ -1565,18 +1565,18 @@
     </row>
     <row r="73" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C73" s="20" t="s">
-        <v>147</v>
+        <v>170</v>
       </c>
     </row>
     <row r="74" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="E74" s="1" t="s">
         <v>0</v>
@@ -1587,7 +1587,7 @@
     </row>
     <row r="75" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>0</v>
@@ -1598,7 +1598,7 @@
     </row>
     <row r="76" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>0</v>
@@ -1609,7 +1609,7 @@
     </row>
     <row r="77" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>0</v>
@@ -1620,7 +1620,7 @@
     </row>
     <row r="78" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="E78" s="1" t="s">
         <v>0</v>
@@ -1631,7 +1631,7 @@
     </row>
     <row r="79" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>0</v>
@@ -1642,7 +1642,7 @@
     </row>
     <row r="80" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="E80" s="1" t="s">
         <v>0</v>
@@ -1653,7 +1653,7 @@
     </row>
     <row r="81" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E81" s="1" t="s">
         <v>0</v>
@@ -1664,24 +1664,24 @@
     </row>
     <row r="82" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C82" s="20" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="83" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C83" s="20" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="84" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1695,7 +1695,7 @@
         <v>126</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="C87" s="4" t="b">
         <v>0</v>
@@ -1712,7 +1712,7 @@
         <v>45</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="C88" s="4" t="b">
         <v>0</v>
@@ -2032,7 +2032,7 @@
         <v>1</v>
       </c>
       <c r="E109" s="6" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F109" s="4" t="b">
         <v>1</v>
@@ -2243,7 +2243,7 @@
     </row>
     <row r="148" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B148" s="29" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="C148" s="28" t="b">
         <v>0</v>
@@ -2251,7 +2251,7 @@
     </row>
     <row r="149" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B149" s="29" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="C149" s="28" t="b">
         <v>0</v>
@@ -2259,7 +2259,7 @@
     </row>
     <row r="150" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B150" s="29" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="C150" s="28" t="b">
         <v>0</v>
@@ -2267,7 +2267,7 @@
     </row>
     <row r="151" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B151" s="29" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="C151" s="28" t="b">
         <v>0</v>
@@ -2275,7 +2275,7 @@
     </row>
     <row r="152" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B152" s="29" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C152" s="28" t="b">
         <v>0</v>
@@ -2283,7 +2283,7 @@
     </row>
     <row r="153" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B153" s="29" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="C153" s="28" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Changes made untill Feb 28 -Marijke
</commit_message>
<xml_diff>
--- a/ConfigFiles/ConfigTest.xlsx
+++ b/ConfigFiles/ConfigTest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24527"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Github\DARKO\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marij\OneDrive\Documenten\1. School\2021-2022\BP\DARKO\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEC47018-159F-421D-972D-520B1CE43234}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{167B134D-8702-46D9-9C30-A4A95B9E0FD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -1081,23 +1081,23 @@
   <dimension ref="A1:H166"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="C84" sqref="C84"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="30.28515625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="68.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="2.42578125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="96.28515625" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="30.26953125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.453125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="68.7265625" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.1796875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.453125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7265625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="2.453125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="96.26953125" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="32" t="s">
         <v>118</v>
       </c>
@@ -1109,7 +1109,7 @@
       <c r="G1" s="32"/>
       <c r="H1" s="32"/>
     </row>
-    <row r="2" spans="1:8" ht="3" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="3" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -1119,8 +1119,8 @@
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="31" t="s">
         <v>119</v>
       </c>
@@ -1131,7 +1131,7 @@
       <c r="G4" s="31"/>
       <c r="H4" s="31"/>
     </row>
-    <row r="5" spans="1:8" s="8" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" s="8" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="7"/>
       <c r="B5" s="16"/>
       <c r="C5" s="16"/>
@@ -1141,7 +1141,7 @@
       <c r="G5" s="16"/>
       <c r="H5" s="16"/>
     </row>
-    <row r="6" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>44</v>
       </c>
@@ -1155,7 +1155,7 @@
       <c r="G6" s="30"/>
       <c r="H6" s="30"/>
     </row>
-    <row r="7" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
       <c r="D7" s="12"/>
@@ -1164,20 +1164,20 @@
       <c r="G7" s="12"/>
       <c r="H7" s="12"/>
     </row>
-    <row r="8" spans="1:8" s="8" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" s="8" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="7"/>
       <c r="C8" s="14"/>
     </row>
-    <row r="9" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="10" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="11" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="12" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="13" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="14" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="15" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="16" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>34</v>
       </c>
@@ -1192,7 +1192,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>31</v>
       </c>
@@ -1206,7 +1206,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>32</v>
       </c>
@@ -1220,7 +1220,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>33</v>
       </c>
@@ -1234,7 +1234,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>65</v>
       </c>
@@ -1245,7 +1245,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>100</v>
       </c>
@@ -1257,17 +1257,17 @@
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:8" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="25" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="26" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="27" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="28" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="29" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="30" spans="1:8" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="7"/>
       <c r="C30" s="14"/>
     </row>
-    <row r="31" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>37</v>
       </c>
@@ -1281,7 +1281,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
         <v>38</v>
       </c>
@@ -1295,7 +1295,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>41</v>
       </c>
@@ -1309,7 +1309,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>43</v>
       </c>
@@ -1320,24 +1320,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="1:8" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="36" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="37" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="38" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="39" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="40" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="41" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="42" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="43" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="44" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="45" spans="1:8" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="7"/>
       <c r="C45" s="14"/>
     </row>
-    <row r="46" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C46" s="1"/>
     </row>
-    <row r="47" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="2" t="s">
         <v>39</v>
       </c>
@@ -1351,7 +1351,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
         <v>50</v>
       </c>
@@ -1365,26 +1365,26 @@
         <v>52</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="50" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="52" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="53" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="54" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="55" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="56" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="57" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="58" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="59" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="60" spans="1:8" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="50" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="51" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="52" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="53" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="54" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="55" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="56" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="57" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="58" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="59" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="60" spans="1:8" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="9"/>
       <c r="C60" s="15"/>
     </row>
-    <row r="61" spans="1:8" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="7"/>
       <c r="C61" s="14"/>
     </row>
-    <row r="62" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="2" t="s">
         <v>134</v>
       </c>
@@ -1401,7 +1401,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" s="2" t="s">
         <v>135</v>
       </c>
@@ -1418,7 +1418,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="2" t="s">
         <v>136</v>
       </c>
@@ -1435,7 +1435,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="65" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" s="2" t="s">
         <v>137</v>
       </c>
@@ -1453,7 +1453,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" s="2" t="s">
         <v>128</v>
       </c>
@@ -1470,7 +1470,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" s="2" t="s">
         <v>129</v>
       </c>
@@ -1487,7 +1487,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" s="2" t="s">
         <v>123</v>
       </c>
@@ -1505,7 +1505,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" s="2" t="s">
         <v>131</v>
       </c>
@@ -1523,7 +1523,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="70" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" s="2" t="s">
         <v>132</v>
       </c>
@@ -1535,7 +1535,7 @@
       </c>
       <c r="D70" s="19"/>
     </row>
-    <row r="71" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" s="2" t="s">
         <v>133</v>
       </c>
@@ -1549,7 +1549,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" s="2" t="s">
         <v>141</v>
       </c>
@@ -1563,7 +1563,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A73" s="2" t="s">
         <v>143</v>
       </c>
@@ -1574,7 +1574,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A74" s="2" t="s">
         <v>150</v>
       </c>
@@ -1585,7 +1585,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="75" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A75" s="2" t="s">
         <v>151</v>
       </c>
@@ -1596,7 +1596,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="76" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A76" s="2" t="s">
         <v>148</v>
       </c>
@@ -1607,7 +1607,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A77" s="2" t="s">
         <v>149</v>
       </c>
@@ -1618,7 +1618,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A78" s="2" t="s">
         <v>146</v>
       </c>
@@ -1629,7 +1629,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A79" s="2" t="s">
         <v>147</v>
       </c>
@@ -1640,7 +1640,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A80" s="2" t="s">
         <v>144</v>
       </c>
@@ -1651,7 +1651,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="81" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A81" s="2" t="s">
         <v>145</v>
       </c>
@@ -1662,7 +1662,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="82" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A82" s="2" t="s">
         <v>160</v>
       </c>
@@ -1673,7 +1673,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A83" s="2" t="s">
         <v>161</v>
       </c>
@@ -1684,13 +1684,13 @@
         <v>172</v>
       </c>
     </row>
-    <row r="84" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="85" spans="1:6" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="85" spans="1:6" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A85" s="9"/>
       <c r="C85" s="15"/>
     </row>
-    <row r="86" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="87" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="87" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A87" s="22" t="s">
         <v>126</v>
       </c>
@@ -1707,7 +1707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A88" s="31" t="s">
         <v>45</v>
       </c>
@@ -1724,7 +1724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A89" s="31"/>
       <c r="B89" s="6" t="s">
         <v>20</v>
@@ -1739,7 +1739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A90" s="31"/>
       <c r="B90" s="6" t="s">
         <v>106</v>
@@ -1754,7 +1754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A91" s="31"/>
       <c r="B91" s="6" t="s">
         <v>101</v>
@@ -1769,7 +1769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A92" s="31"/>
       <c r="B92" s="6" t="s">
         <v>3</v>
@@ -1784,7 +1784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A93" s="31"/>
       <c r="B93" s="6" t="s">
         <v>114</v>
@@ -1799,7 +1799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A94" s="31"/>
       <c r="B94" s="6" t="s">
         <v>29</v>
@@ -1814,7 +1814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A95" s="31"/>
       <c r="B95" s="6" t="s">
         <v>14</v>
@@ -1829,7 +1829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A96" s="31"/>
       <c r="B96" s="6" t="s">
         <v>4</v>
@@ -1844,7 +1844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A97" s="31"/>
       <c r="B97" s="6" t="s">
         <v>6</v>
@@ -1859,7 +1859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A98" s="31"/>
       <c r="B98" s="6" t="s">
         <v>5</v>
@@ -1874,7 +1874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A99" s="31"/>
       <c r="B99" s="6" t="s">
         <v>7</v>
@@ -1889,7 +1889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A100" s="31"/>
       <c r="B100" s="6" t="s">
         <v>9</v>
@@ -1904,7 +1904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A101" s="31"/>
       <c r="B101" s="6" t="s">
         <v>10</v>
@@ -1919,7 +1919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A102" s="31"/>
       <c r="B102" s="6" t="s">
         <v>26</v>
@@ -1934,7 +1934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B103" s="6" t="s">
         <v>11</v>
       </c>
@@ -1948,7 +1948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B104" s="6" t="s">
         <v>12</v>
       </c>
@@ -1962,7 +1962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B105" s="6" t="s">
         <v>18</v>
       </c>
@@ -1976,7 +1976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B106" s="6" t="s">
         <v>8</v>
       </c>
@@ -1993,7 +1993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B107" s="6" t="s">
         <v>111</v>
       </c>
@@ -2010,7 +2010,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="108" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B108" s="6" t="s">
         <v>13</v>
       </c>
@@ -2024,7 +2024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B109" s="6" t="s">
         <v>130</v>
       </c>
@@ -2038,17 +2038,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:8" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A110" s="9"/>
       <c r="C110" s="15"/>
     </row>
-    <row r="111" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="112" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="112" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A112" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="113" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A113" s="2" t="s">
         <v>1</v>
       </c>
@@ -2059,7 +2059,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A114" s="2" t="s">
         <v>59</v>
       </c>
@@ -2073,7 +2073,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="115" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A115" s="2" t="s">
         <v>60</v>
       </c>
@@ -2087,7 +2087,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="116" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A116" s="2" t="s">
         <v>62</v>
       </c>
@@ -2098,30 +2098,30 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="118" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="119" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="120" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="121" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="122" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="123" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="124" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="125" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="126" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="127" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="128" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="129" spans="1:3" s="10" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="118" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="119" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="120" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="121" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="122" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="123" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="124" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="125" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="126" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="127" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="128" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="129" spans="1:3" s="10" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A129" s="9"/>
       <c r="C129" s="15"/>
     </row>
-    <row r="130" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="131" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="131" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A131" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="132" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="133" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="133" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B133" s="24" t="s">
         <v>70</v>
       </c>
@@ -2129,7 +2129,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B134" s="24" t="s">
         <v>71</v>
       </c>
@@ -2137,7 +2137,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B135" s="24" t="s">
         <v>72</v>
       </c>
@@ -2145,7 +2145,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B136" s="24" t="s">
         <v>73</v>
       </c>
@@ -2153,7 +2153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B137" s="24" t="s">
         <v>74</v>
       </c>
@@ -2161,7 +2161,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B138" s="24" t="s">
         <v>75</v>
       </c>
@@ -2169,7 +2169,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B139" s="24" t="s">
         <v>76</v>
       </c>
@@ -2177,7 +2177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B140" s="24" t="s">
         <v>77</v>
       </c>
@@ -2185,7 +2185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B141" s="24" t="s">
         <v>78</v>
       </c>
@@ -2193,7 +2193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B142" s="24" t="s">
         <v>79</v>
       </c>
@@ -2201,7 +2201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B143" s="24" t="s">
         <v>80</v>
       </c>
@@ -2209,7 +2209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B144" s="24" t="s">
         <v>81</v>
       </c>
@@ -2217,7 +2217,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B145" s="24" t="s">
         <v>82</v>
       </c>
@@ -2225,7 +2225,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B146" s="29" t="s">
         <v>83</v>
       </c>
@@ -2233,7 +2233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B147" s="24" t="s">
         <v>84</v>
       </c>
@@ -2241,7 +2241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B148" s="29" t="s">
         <v>154</v>
       </c>
@@ -2249,7 +2249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B149" s="29" t="s">
         <v>155</v>
       </c>
@@ -2257,7 +2257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B150" s="29" t="s">
         <v>156</v>
       </c>
@@ -2265,7 +2265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B151" s="29" t="s">
         <v>157</v>
       </c>
@@ -2273,7 +2273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B152" s="29" t="s">
         <v>158</v>
       </c>
@@ -2281,7 +2281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B153" s="29" t="s">
         <v>159</v>
       </c>
@@ -2289,7 +2289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="166" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F166" s="2"/>
     </row>
   </sheetData>
@@ -2391,14 +2391,14 @@
       <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="2" width="32.5703125" customWidth="1"/>
+    <col min="1" max="1" width="23.7265625" customWidth="1"/>
+    <col min="2" max="2" width="32.54296875" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
         <v>2</v>
       </c>
@@ -2409,7 +2409,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="b">
         <v>1</v>
       </c>
@@ -2420,7 +2420,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="b">
         <v>0</v>
       </c>
@@ -2440,12 +2440,12 @@
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="17"/>
+    <col min="1" max="1" width="9.1796875" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="26"/>
       <c r="B1" s="26" t="s">
         <v>85</v>
@@ -2490,7 +2490,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="26" t="s">
         <v>70</v>
       </c>
@@ -2537,7 +2537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="26" t="s">
         <v>71</v>
       </c>
@@ -2584,7 +2584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" s="26" t="s">
         <v>72</v>
       </c>
@@ -2631,7 +2631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" s="26" t="s">
         <v>73</v>
       </c>
@@ -2678,7 +2678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" s="26" t="s">
         <v>74</v>
       </c>
@@ -2725,7 +2725,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" s="26" t="s">
         <v>75</v>
       </c>
@@ -2772,7 +2772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" s="26" t="s">
         <v>76</v>
       </c>
@@ -2819,7 +2819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" s="26" t="s">
         <v>77</v>
       </c>
@@ -2866,7 +2866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" s="26" t="s">
         <v>78</v>
       </c>
@@ -2913,7 +2913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" s="26" t="s">
         <v>79</v>
       </c>
@@ -2960,7 +2960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" s="26" t="s">
         <v>80</v>
       </c>
@@ -3007,7 +3007,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13" s="26" t="s">
         <v>81</v>
       </c>
@@ -3054,7 +3054,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" s="26" t="s">
         <v>82</v>
       </c>
@@ -3101,7 +3101,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15" s="26" t="s">
         <v>83</v>
       </c>
@@ -3148,7 +3148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16" s="26" t="s">
         <v>84</v>
       </c>

</xml_diff>